<commit_message>
completing all code, remaining optimization and explanantion
</commit_message>
<xml_diff>
--- a/ComparingCalciumAndElectrophysiologyMapping/velocity_amplitude_results.xlsx
+++ b/ComparingCalciumAndElectrophysiologyMapping/velocity_amplitude_results.xlsx
@@ -16,16 +16,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Button (Mean: 2.27, Median: 1.88, Std: 1.22)</t>
+    <t>Button (Mean: 2.92, Median: 2.13, Std: 2.16)</t>
   </si>
   <si>
-    <t>Calcium (Mean: 2.35, Median: 2.04, Std: 1.33)</t>
+    <t>Calcium (Mean: 3.33, Median: 2.54, Std: 2.52)</t>
   </si>
   <si>
-    <t>Top (Mean: 2.33, Median: 2.16, Std: 1.08)</t>
+    <t>Top (Mean: 3.49, Median: 2.93, Std: 2.19)</t>
   </si>
   <si>
-    <t>Mean (Mean: 2.95, Median: 2.52, Std: 1.68)</t>
+    <t>Mean (Mean: 4.06, Median: 2.66, Std: 3.62)</t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D248"/>
+  <dimension ref="A1:D260"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -405,3439 +405,3607 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>1.284444444444447</v>
+        <v>5.792307288226756</v>
       </c>
       <c r="B2">
-        <v>1.060987253150476</v>
+        <v>1.056743304137876</v>
       </c>
       <c r="C2">
-        <v>0.5705463954824479</v>
+        <v>0.56826420990052</v>
       </c>
       <c r="D2">
-        <v>1.01838095238095</v>
+        <v>1.014307428571428</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>3.005645368574345</v>
+        <v>5.782929363806535</v>
       </c>
       <c r="B3">
-        <v>1.407948717948721</v>
+        <v>1.402316923076928</v>
       </c>
       <c r="C3">
-        <v>0.8019393254333356</v>
+        <v>0.7987315681316033</v>
       </c>
       <c r="D3">
-        <v>1.372828933323154</v>
+        <v>1.367337617589864</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>3.92964437180882</v>
+        <v>3.91392579432159</v>
       </c>
       <c r="B4">
-        <v>2.119333333333337</v>
+        <v>4.017561692680682</v>
       </c>
       <c r="C4">
-        <v>1.414995623505768</v>
+        <v>1.409335641011738</v>
       </c>
       <c r="D4">
-        <v>2.022104667266022</v>
+        <v>2.014016248596954</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>4.08707719525826</v>
+        <v>4.070728886477197</v>
       </c>
       <c r="B5">
-        <v>2.312</v>
+        <v>5.815326980681761</v>
       </c>
       <c r="C5">
-        <v>1.502822684287198</v>
+        <v>1.496811393550039</v>
       </c>
       <c r="D5">
-        <v>2.057680901997302</v>
+        <v>2.049450178389305</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
-        <v>5.779999999999919</v>
+        <v>6.436387509154347</v>
       </c>
       <c r="B6">
-        <v>2.312</v>
+        <v>5.870888691482436</v>
       </c>
       <c r="C6">
-        <v>2.94723327885664</v>
+        <v>2.935444345741168</v>
       </c>
       <c r="D6">
-        <v>4.115361803994647</v>
+        <v>4.098900356778612</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>5.780000000000022</v>
+        <v>6.436387509154325</v>
       </c>
       <c r="B7">
-        <v>2.312</v>
+        <v>2.302751999999996</v>
       </c>
       <c r="C7">
-        <v>2.978943814508771</v>
+        <v>2.967028039250691</v>
       </c>
       <c r="D7">
-        <v>4.308157636649626</v>
+        <v>4.290925006102979</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>1.634830878103298</v>
+        <v>1.628291554590888</v>
       </c>
       <c r="B8">
-        <v>5.780000000000022</v>
+        <v>8.141457772954467</v>
       </c>
       <c r="C8">
-        <v>1.926666666666662</v>
+        <v>5.836288992570767</v>
       </c>
       <c r="D8">
-        <v>5.780000000000022</v>
+        <v>11.86811215700255</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
-        <v>1.319159200589777</v>
+        <v>1.362505725988525</v>
       </c>
       <c r="B9">
-        <v>1.926666666666668</v>
+        <v>8.581850012205917</v>
       </c>
       <c r="C9">
-        <v>3.04632747929555</v>
+        <v>1.995748524733533</v>
       </c>
       <c r="D9">
-        <v>3.9409090909091</v>
+        <v>4.029815999999962</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
-        <v>0.8027777777777789</v>
+        <v>0.8897958357082806</v>
       </c>
       <c r="B10">
-        <v>1.789047619047619</v>
+        <v>6.436387509154529</v>
       </c>
       <c r="C10">
-        <v>3.231118227487208</v>
+        <v>3.218193754577265</v>
       </c>
       <c r="D10">
-        <v>1.78673862592024</v>
+        <v>2.007762168374429</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
-        <v>0.963333333333331</v>
+        <v>0.9594799999999996</v>
       </c>
       <c r="B11">
-        <v>1.274576607286027</v>
+        <v>1.644822857142858</v>
       </c>
       <c r="C11">
-        <v>0.8799705256166125</v>
+        <v>0.8764506435141494</v>
       </c>
       <c r="D11">
-        <v>0.6248648648648645</v>
+        <v>0.6223654054054057</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
-        <v>0.7128150230716386</v>
+        <v>4.172360222093414</v>
       </c>
       <c r="B12">
-        <v>1.651428571428571</v>
+        <v>3.991497049466804</v>
       </c>
       <c r="C12">
-        <v>1.032924378942567</v>
+        <v>1.028792681426797</v>
       </c>
       <c r="D12">
-        <v>1.199453677924185</v>
+        <v>1.194655863212473</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13">
-        <v>1.605555555555554</v>
+        <v>0.7995666666666685</v>
       </c>
       <c r="B13">
-        <v>1.981714285714287</v>
+        <v>2.535768571428586</v>
       </c>
       <c r="C13">
-        <v>1.347015631774519</v>
+        <v>1.341627569247414</v>
       </c>
       <c r="D13">
-        <v>2.209327747989194</v>
+        <v>2.200490436997254</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14">
-        <v>1.789047619047619</v>
+        <v>4.017561692680681</v>
       </c>
       <c r="B14">
-        <v>2.312</v>
+        <v>3.991497049466673</v>
       </c>
       <c r="C14">
-        <v>1.740676959627426</v>
+        <v>1.733714251788918</v>
       </c>
       <c r="D14">
-        <v>2.933459310098812</v>
+        <v>2.921725472858447</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15">
-        <v>2.601000000000005</v>
+        <v>4.208607844227844</v>
       </c>
       <c r="B15">
-        <v>1.926666666666674</v>
+        <v>0.9868937142857175</v>
       </c>
       <c r="C15">
-        <v>1.464428126692874</v>
+        <v>1.458570414186112</v>
       </c>
       <c r="D15">
-        <v>2.112754941881446</v>
+        <v>4.365963479325177</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16">
-        <v>5.780000000000022</v>
+        <v>6.918908675564413</v>
       </c>
       <c r="B16">
-        <v>2.154078818324795</v>
+        <v>5.870888691482437</v>
       </c>
       <c r="C16">
-        <v>1.541333333333332</v>
+        <v>1.535168</v>
       </c>
       <c r="D16">
-        <v>1.878499999999995</v>
+        <v>4.035523149156272</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
-        <v>5.77999999999997</v>
+        <v>5.427638515302978</v>
       </c>
       <c r="B17">
-        <v>3.853333333333324</v>
+        <v>5.836288992570566</v>
       </c>
       <c r="C17">
-        <v>1.878499999999997</v>
+        <v>1.870986000000004</v>
       </c>
       <c r="D17">
-        <v>4.335000000000016</v>
+        <v>8.197800713557044</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18">
-        <v>4.816666666666673</v>
+        <v>4.995852239359283</v>
       </c>
       <c r="B18">
-        <v>4.816666666666673</v>
+        <v>2.145462503051507</v>
       </c>
       <c r="C18">
-        <v>2.889999999999993</v>
+        <v>2.398699999999998</v>
       </c>
       <c r="D18">
-        <v>3.853333333333324</v>
+        <v>9.225211567418993</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19">
-        <v>2.006366361188463</v>
+        <v>1.998340895743713</v>
       </c>
       <c r="B19">
-        <v>4.08707719525826</v>
+        <v>1.279306666666674</v>
       </c>
       <c r="C19">
-        <v>3.853333333333322</v>
+        <v>4.562551363766087</v>
       </c>
       <c r="D19">
-        <v>4.087077195258259</v>
+        <v>2.558613333333317</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20">
-        <v>1.908456673226502</v>
+        <v>1.900822846533599</v>
       </c>
       <c r="B20">
-        <v>5.780000000000022</v>
+        <v>4.995852239359305</v>
       </c>
       <c r="C20">
-        <v>2.408333333333351</v>
+        <v>5.26075980528474</v>
       </c>
       <c r="D20">
-        <v>3.159968283947767</v>
+        <v>5.465200475704816</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21">
-        <v>1.487718555372625</v>
+        <v>1.49247952517673</v>
       </c>
       <c r="B21">
-        <v>4.08707719525826</v>
+        <v>4.070728886477234</v>
       </c>
       <c r="C21">
-        <v>2.724718130172189</v>
+        <v>5.27471651422354</v>
       </c>
       <c r="D21">
-        <v>3.473347728696983</v>
+        <v>5.187570102965997</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22">
-        <v>1.431238095238096</v>
+        <v>1.425513142857142</v>
       </c>
       <c r="B22">
-        <v>1.046065707471908</v>
+        <v>6.436387509154529</v>
       </c>
       <c r="C22">
-        <v>1.085001842268154</v>
+        <v>8.141457772954467</v>
       </c>
       <c r="D22">
-        <v>2.408333333333333</v>
+        <v>5.465200475704862</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23">
-        <v>1.046065707471909</v>
+        <v>1.041881444642019</v>
       </c>
       <c r="B23">
-        <v>1.651428571428571</v>
+        <v>4.070728886477234</v>
       </c>
       <c r="C23">
-        <v>1.743156695627282</v>
+        <v>1.080661834899083</v>
       </c>
       <c r="D23">
-        <v>0.9358095238095234</v>
+        <v>2.398700000000013</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24">
-        <v>1.272864756282838</v>
+        <v>1.31359309978478</v>
       </c>
       <c r="B24">
-        <v>2.219040465960244</v>
+        <v>4.257165360109903</v>
       </c>
       <c r="C24">
-        <v>2.465434558267263</v>
+        <v>1.736184068844771</v>
       </c>
       <c r="D24">
-        <v>1.167676767676768</v>
+        <v>0.9594799999999983</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25">
-        <v>1.533147290629452</v>
+        <v>3.70671661559178</v>
       </c>
       <c r="B25">
-        <v>2.265959829321293</v>
+        <v>5.815326980681711</v>
       </c>
       <c r="C25">
-        <v>2.114641546156852</v>
+        <v>2.455572820034192</v>
       </c>
       <c r="D25">
-        <v>1.467230769230771</v>
+        <v>3.915453737373758</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26">
-        <v>2.507957951485585</v>
+        <v>4.481141405724684</v>
       </c>
       <c r="B26">
-        <v>2.154078818324792</v>
+        <v>4.395287070652408</v>
       </c>
       <c r="C26">
-        <v>1.605555555555556</v>
+        <v>2.106182979972227</v>
       </c>
       <c r="D26">
-        <v>2.408333333333341</v>
+        <v>3.959643405930754</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27">
-        <v>3.04632747929555</v>
+        <v>4.196011293049641</v>
       </c>
       <c r="B27">
-        <v>1.284444444444447</v>
+        <v>4.408624744906671</v>
       </c>
       <c r="C27">
-        <v>2.40833333333333</v>
+        <v>1.599133333333333</v>
       </c>
       <c r="D27">
-        <v>2.686075632564152</v>
+        <v>2.398700000000006</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28">
-        <v>2.890000000000011</v>
+        <v>7.735575064337398</v>
       </c>
       <c r="B28">
-        <v>2.030884986197022</v>
+        <v>3.034142169378371</v>
       </c>
       <c r="C28">
-        <v>2.311999999999992</v>
+        <v>4.157746666666624</v>
       </c>
       <c r="D28">
-        <v>6.74333333333329</v>
+        <v>2.675331330033896</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29">
-        <v>5.780000000000022</v>
+        <v>8.635319999999844</v>
       </c>
       <c r="B29">
-        <v>4.08707719525826</v>
+        <v>5.792307288226756</v>
       </c>
       <c r="C29">
-        <v>3.473347728696961</v>
+        <v>5.870888691482337</v>
       </c>
       <c r="D29">
-        <v>7.706666666666741</v>
+        <v>8.88634810599801</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30">
-        <v>3.853333333333324</v>
+        <v>3.837920000000021</v>
       </c>
       <c r="B30">
-        <v>5.780000000000022</v>
+        <v>2.022761446252248</v>
       </c>
       <c r="C30">
-        <v>4.308157636649573</v>
+        <v>3.218193754577239</v>
       </c>
       <c r="D30">
-        <v>4.816666666666599</v>
+        <v>12.87277501830869</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31">
-        <v>2.592064899736209</v>
+        <v>2.581696640137236</v>
       </c>
       <c r="B31">
-        <v>5.780000000000022</v>
+        <v>2.713819257651561</v>
       </c>
       <c r="C31">
-        <v>1.436052545549889</v>
+        <v>5.189181506673261</v>
       </c>
       <c r="D31">
-        <v>4.6490191199626</v>
+        <v>14.39219999999967</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32">
-        <v>2.605010796522732</v>
+        <v>2.594590753336627</v>
       </c>
       <c r="B32">
-        <v>5.77999999999997</v>
+        <v>5.427638515302954</v>
       </c>
       <c r="C32">
-        <v>3.85333333333337</v>
+        <v>6.91890867556432</v>
       </c>
       <c r="D32">
-        <v>3.97060036026829</v>
+        <v>6.918908675564413</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33">
-        <v>1.880968463614184</v>
+        <v>1.873444589759733</v>
       </c>
       <c r="B33">
-        <v>0.7489533767156852</v>
+        <v>6.918908675564413</v>
       </c>
       <c r="C33">
-        <v>2.924001169670893</v>
+        <v>3.867787532168716</v>
       </c>
       <c r="D33">
-        <v>2.889999999999998</v>
+        <v>5.452177032637192</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34">
-        <v>1.634961200625577</v>
+        <v>1.628421355823072</v>
       </c>
       <c r="B34">
-        <v>1.567864254643128</v>
+        <v>3.83792000000002</v>
       </c>
       <c r="C34">
-        <v>2.098622886828484</v>
+        <v>1.279306666666674</v>
       </c>
       <c r="D34">
-        <v>3.892454471674465</v>
+        <v>5.303774455866453</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35">
-        <v>1.245645498229347</v>
+        <v>1.24066291623643</v>
       </c>
       <c r="B35">
-        <v>3.025272358946389</v>
+        <v>5.427638515302954</v>
       </c>
       <c r="C35">
-        <v>1.467936507936507</v>
+        <v>2.912305164992189</v>
       </c>
       <c r="D35">
-        <v>3.922612289738933</v>
+        <v>4.290925006102895</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36">
-        <v>1.363210273582179</v>
+        <v>1.657623228072316</v>
       </c>
       <c r="B36">
-        <v>3.055142857142843</v>
+        <v>0.6788787162439255</v>
       </c>
       <c r="C36">
-        <v>1.789047619047621</v>
+        <v>4.356642474412113</v>
       </c>
       <c r="D36">
-        <v>3.231697610699951</v>
+        <v>5.785592796571672</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37">
-        <v>1.578440083058269</v>
+        <v>1.692671992503003</v>
       </c>
       <c r="B37">
-        <v>2.246860130147052</v>
+        <v>3.894195443760625</v>
       </c>
       <c r="C37">
-        <v>2.119333333333334</v>
+        <v>3.95975873015875</v>
       </c>
       <c r="D37">
-        <v>2.726420547164361</v>
+        <v>4.848724160857294</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38">
-        <v>1.944048674802152</v>
+        <v>1.936272480102946</v>
       </c>
       <c r="B38">
-        <v>3.853333333333324</v>
+        <v>3.013171269510608</v>
       </c>
       <c r="C38">
-        <v>4.33500000000001</v>
+        <v>4.017561692680811</v>
       </c>
       <c r="D38">
-        <v>3.058983857486478</v>
+        <v>3.218770820257163</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39">
-        <v>2.592064899736204</v>
+        <v>4.507769380126295</v>
       </c>
       <c r="B39">
-        <v>2.246860130147052</v>
+        <v>3.013171269510608</v>
       </c>
       <c r="C39">
-        <v>3.853333333333324</v>
+        <v>4.087780184736855</v>
       </c>
       <c r="D39">
-        <v>7.706666666666558</v>
+        <v>2.715514864975698</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40">
-        <v>2.889999999999985</v>
+        <v>5.934056078501285</v>
       </c>
       <c r="B40">
-        <v>3.473347728696983</v>
+        <v>3.890859328380377</v>
       </c>
       <c r="C40">
-        <v>3.853333333333324</v>
+        <v>4.317659999999991</v>
       </c>
       <c r="D40">
-        <v>5.44943626034425</v>
+        <v>3.046747922056522</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41">
-        <v>2.889999999999985</v>
+        <v>11.51375999999965</v>
       </c>
       <c r="B41">
-        <v>3.744766883578416</v>
+        <v>7.675840000000019</v>
       </c>
       <c r="C41">
-        <v>1.284444444444441</v>
+        <v>6.068284338756742</v>
       </c>
       <c r="D41">
-        <v>5.744210182199487</v>
+        <v>9.594800000000097</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42">
-        <v>2.588880543620319</v>
+        <v>2.878440000000015</v>
       </c>
       <c r="B42">
-        <v>4.308157636649611</v>
+        <v>2.23787268962648</v>
       </c>
       <c r="C42">
-        <v>3.853333333333347</v>
+        <v>7.67584000000003</v>
       </c>
       <c r="D42">
-        <v>4.624000000000001</v>
+        <v>5.427638515302914</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43">
-        <v>2.724718130172173</v>
+        <v>2.57852502144583</v>
       </c>
       <c r="B43">
-        <v>4.08707719525826</v>
+        <v>3.4594543377822</v>
       </c>
       <c r="C43">
-        <v>3.744766883578435</v>
+        <v>3.837920000000015</v>
       </c>
       <c r="D43">
-        <v>5.202000000000011</v>
+        <v>3.492559918283455</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44">
-        <v>2.408333333333329</v>
+        <v>2.713819257651457</v>
       </c>
       <c r="B44">
-        <v>5.779999999999919</v>
+        <v>4.939225603837125</v>
       </c>
       <c r="C44">
-        <v>5.779999999999919</v>
+        <v>4.612605783709545</v>
       </c>
       <c r="D44">
-        <v>3.963428571428582</v>
+        <v>6.918908675564309</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45">
-        <v>2.324509559981295</v>
+        <v>2.3987</v>
       </c>
       <c r="B45">
-        <v>2.096150883423489</v>
+        <v>5.18918150667331</v>
       </c>
       <c r="C45">
-        <v>1.444999999999999</v>
+        <v>4.939225603837127</v>
       </c>
       <c r="D45">
-        <v>2.889999999999985</v>
+        <v>5.181192000000012</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46">
-        <v>2.096150883423491</v>
+        <v>2.315211521741379</v>
       </c>
       <c r="B46">
-        <v>2.545952380952403</v>
+        <v>6.068284338756618</v>
       </c>
       <c r="C46">
-        <v>2.27071428571429</v>
+        <v>6.436387509154529</v>
       </c>
       <c r="D46">
-        <v>2.096150883423489</v>
+        <v>8.114459428571728</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47">
-        <v>1.362359065086078</v>
+        <v>2.087766279889811</v>
       </c>
       <c r="B47">
-        <v>2.569093670976086</v>
+        <v>6.436387509154325</v>
       </c>
       <c r="C47">
-        <v>2.507957951485587</v>
+        <v>5.792307288226756</v>
       </c>
       <c r="D47">
-        <v>2.097480530374102</v>
+        <v>11.6033625965067</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48">
-        <v>1.69946987199097</v>
+        <v>1.356909628825737</v>
       </c>
       <c r="B48">
-        <v>2.154078818324813</v>
+        <v>2.087766279889811</v>
       </c>
       <c r="C48">
-        <v>2.817006589175255</v>
+        <v>5.840858373364056</v>
       </c>
       <c r="D48">
-        <v>2.043538597629121</v>
+        <v>1.815110858442424</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49">
-        <v>2.344830291472076</v>
+        <v>1.692671992503003</v>
       </c>
       <c r="B49">
-        <v>2.057680901997301</v>
+        <v>2.535768571428579</v>
       </c>
       <c r="C49">
-        <v>3.473347728696983</v>
+        <v>4.481141405724673</v>
       </c>
       <c r="D49">
-        <v>2.812416204445826</v>
+        <v>1.931427757691158</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50">
-        <v>1.736673864348481</v>
+        <v>2.335450970306187</v>
       </c>
       <c r="B50">
-        <v>1.444999999999999</v>
+        <v>2.558817296292193</v>
       </c>
       <c r="C50">
-        <v>4.816666666666673</v>
+        <v>2.805738562818548</v>
       </c>
       <c r="D50">
-        <v>3.853333333333279</v>
+        <v>2.035364443238608</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51">
-        <v>3.853333333333324</v>
+        <v>1.729727168891103</v>
       </c>
       <c r="B51">
-        <v>0.9088068490547883</v>
+        <v>3.261604828601339</v>
       </c>
       <c r="C51">
-        <v>4.33500000000001</v>
+        <v>5.897312343922266</v>
       </c>
       <c r="D51">
-        <v>5.78000000000001</v>
+        <v>2.801166539628044</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52">
-        <v>3.853333333333324</v>
+        <v>3.837920000000021</v>
       </c>
       <c r="B52">
-        <v>1.953242634729104</v>
+        <v>5.139665283425037</v>
       </c>
       <c r="C52">
-        <v>3.371666666666661</v>
+        <v>4.797399999999989</v>
       </c>
       <c r="D52">
-        <v>5.744210182199487</v>
+        <v>11.58461457645325</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53">
-        <v>2.889999999999985</v>
+        <v>7.675840000000042</v>
       </c>
       <c r="B53">
-        <v>3.761936927228353</v>
+        <v>1.439220000000001</v>
       </c>
       <c r="C53">
-        <v>3.761936927228354</v>
+        <v>4.797400000000013</v>
       </c>
       <c r="D53">
-        <v>5.744210182199514</v>
+        <v>5.756879999999986</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54">
-        <v>3.458472509470829</v>
+        <v>0.9594800000000051</v>
       </c>
       <c r="B54">
-        <v>4.087077195258224</v>
+        <v>0.9051716216585719</v>
       </c>
       <c r="C54">
-        <v>3.458472509470833</v>
+        <v>4.797400000000013</v>
       </c>
       <c r="D54">
-        <v>4.624000000000001</v>
+        <v>5.721233341470679</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55">
-        <v>3.084171507696829</v>
+        <v>4.52585810829286</v>
       </c>
       <c r="B55">
-        <v>4.08707719525826</v>
+        <v>4.324317922227758</v>
       </c>
       <c r="C55">
-        <v>2.724718130172173</v>
+        <v>4.939225603837076</v>
       </c>
       <c r="D55">
-        <v>4.624000000000001</v>
+        <v>5.427638515303106</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56">
-        <v>3.240081124670259</v>
+        <v>3.071834821666025</v>
       </c>
       <c r="B56">
-        <v>2.31420158468374</v>
+        <v>3.746889179519452</v>
       </c>
       <c r="C56">
-        <v>2.890000000000004</v>
+        <v>4.290925006102971</v>
       </c>
       <c r="D56">
-        <v>4.238666666666663</v>
+        <v>2.59059599999998</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57">
-        <v>2.588880543620311</v>
+        <v>3.227120800171548</v>
       </c>
       <c r="B57">
-        <v>2.124198034611994</v>
+        <v>4.070728886477234</v>
       </c>
       <c r="C57">
-        <v>3.162577671910075</v>
+        <v>5.27471651422354</v>
       </c>
       <c r="D57">
-        <v>1.922681829584532</v>
+        <v>8.26713268663935</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58">
-        <v>1.610789654379988</v>
+        <v>2.578525021445838</v>
       </c>
       <c r="B58">
-        <v>2.154078818324794</v>
+        <v>6.068284338756746</v>
       </c>
       <c r="C58">
-        <v>3.084171507696825</v>
+        <v>2.805738562818559</v>
       </c>
       <c r="D58">
-        <v>2.063839678443304</v>
+        <v>4.221711999999983</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59">
-        <v>1.57844008305827</v>
+        <v>1.812002967015091</v>
       </c>
       <c r="B59">
-        <v>1.926666666666668</v>
+        <v>2.304944778345017</v>
       </c>
       <c r="C59">
-        <v>3.371666666666661</v>
+        <v>3.227120800171582</v>
       </c>
       <c r="D59">
-        <v>2.608819828621965</v>
+        <v>2.002999171770566</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60">
-        <v>2.371933253932564</v>
+        <v>1.572126322726031</v>
       </c>
       <c r="B60">
-        <v>1.926666666666662</v>
+        <v>2.11570124247354</v>
       </c>
       <c r="C60">
-        <v>2.889999999999998</v>
+        <v>3.07183482166603</v>
       </c>
       <c r="D60">
-        <v>3.148053702286964</v>
+        <v>2.003610649190916</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61">
-        <v>2.507957951485588</v>
+        <v>2.362445520916842</v>
       </c>
       <c r="B61">
-        <v>4.08707719525826</v>
+        <v>2.145462503051497</v>
       </c>
       <c r="C61">
-        <v>3.231118227487179</v>
+        <v>4.443174052999118</v>
       </c>
       <c r="D61">
-        <v>2.890000000000011</v>
+        <v>2.598384549307482</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62">
-        <v>2.890000000000011</v>
+        <v>2.497926119679618</v>
       </c>
       <c r="B62">
-        <v>4.08707719525826</v>
+        <v>4.045522892504494</v>
       </c>
       <c r="C62">
-        <v>3.345763594125851</v>
+        <v>5.934056078501479</v>
       </c>
       <c r="D62">
-        <v>7.706666666666741</v>
+        <v>3.135461487477784</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63">
-        <v>4.08707719525826</v>
+        <v>2.87843999999999</v>
       </c>
       <c r="B63">
-        <v>3.761936927228362</v>
+        <v>5.836288992570566</v>
       </c>
       <c r="C63">
-        <v>2.724718130172173</v>
+        <v>5.897312343922266</v>
       </c>
       <c r="D63">
-        <v>6.16533333333337</v>
+        <v>11.6033625965059</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64">
-        <v>3.458472509470829</v>
+        <v>4.070728886477234</v>
       </c>
       <c r="B64">
-        <v>3.853333333333324</v>
+        <v>2.713819257651489</v>
       </c>
       <c r="C64">
-        <v>2.724718130172157</v>
+        <v>2.92798649554605</v>
       </c>
       <c r="D64">
-        <v>4.238666666666663</v>
+        <v>9.991704478718383</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65">
-        <v>3.405897662715208</v>
+        <v>4.52585810829286</v>
       </c>
       <c r="B65">
-        <v>1.615559113743597</v>
+        <v>4.070728886477197</v>
       </c>
       <c r="C65">
-        <v>2.408333333333338</v>
+        <v>2.549853076100672</v>
       </c>
       <c r="D65">
-        <v>3.853333333333324</v>
+        <v>11.80160400000006</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66">
-        <v>3.473347728696983</v>
+        <v>3.392274072064325</v>
       </c>
       <c r="B66">
-        <v>1.756763202992619</v>
+        <v>3.746889179519442</v>
       </c>
       <c r="C66">
-        <v>3.473347728696975</v>
+        <v>2.713819257651489</v>
       </c>
       <c r="D66">
-        <v>1.425630046143277</v>
+        <v>11.70565600000006</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67">
-        <v>1.046065707471904</v>
+        <v>3.459454337782164</v>
       </c>
       <c r="B67">
-        <v>1.884818966034188</v>
+        <v>6.068284338756746</v>
       </c>
       <c r="C67">
-        <v>2.960498164619607</v>
+        <v>2.713819257651473</v>
       </c>
       <c r="D67">
-        <v>1.911864910929046</v>
+        <v>11.67257798514073</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68">
-        <v>1.322416493664553</v>
+        <v>1.414930122380923</v>
       </c>
       <c r="B68">
-        <v>1.444999999999993</v>
+        <v>1.609096877288625</v>
       </c>
       <c r="C68">
-        <v>2.889999999999998</v>
+        <v>3.459454337782193</v>
       </c>
       <c r="D68">
-        <v>2.412664438840279</v>
+        <v>1.843100892999616</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69">
-        <v>2.023878781883726</v>
+        <v>1.36384567872502</v>
       </c>
       <c r="B69">
-        <v>4.08707719525826</v>
+        <v>1.749736150180653</v>
       </c>
       <c r="C69">
-        <v>3.231118227487188</v>
+        <v>4.632659182769665</v>
       </c>
       <c r="D69">
-        <v>4.022998108100147</v>
+        <v>1.954320980433765</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70">
-        <v>3.046327479295548</v>
+        <v>2.015783266756194</v>
       </c>
       <c r="B70">
-        <v>2.890000000000011</v>
+        <v>1.877279690170063</v>
       </c>
       <c r="C70">
-        <v>2.605010796522756</v>
+        <v>5.934056078501478</v>
       </c>
       <c r="D70">
-        <v>7.706666666666741</v>
+        <v>2.40301378108492</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71">
-        <v>3.853333333333324</v>
+        <v>3.034142169378324</v>
       </c>
       <c r="B71">
-        <v>4.08707719525826</v>
+        <v>5.80168129825315</v>
       </c>
       <c r="C71">
-        <v>3.352498423416835</v>
+        <v>3.218193754577239</v>
       </c>
       <c r="D71">
-        <v>5.449436260344314</v>
+        <v>4.006906115667689</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72">
-        <v>0.8892307692307702</v>
+        <v>11.51376000000006</v>
       </c>
       <c r="B72">
-        <v>0.6745829362043571</v>
+        <v>4.070728886477234</v>
       </c>
       <c r="C72">
-        <v>0.582457169734512</v>
+        <v>2.211492128970851</v>
       </c>
       <c r="D72">
-        <v>4.308157636649544</v>
+        <v>6.918908675564388</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73">
-        <v>1.05090909090909</v>
+        <v>5.756880000000031</v>
       </c>
       <c r="B73">
-        <v>0.8027777777777789</v>
+        <v>2.87843999999999</v>
       </c>
       <c r="C73">
-        <v>0.7128150230716386</v>
+        <v>2.435727326538106</v>
       </c>
       <c r="D73">
-        <v>1.199770122014635</v>
+        <v>5.099706152201299</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74">
-        <v>1.420612572671612</v>
+        <v>6.068284338756746</v>
       </c>
       <c r="B74">
-        <v>1.420612572671612</v>
+        <v>4.070728886477197</v>
       </c>
       <c r="C74">
-        <v>3.231118227487205</v>
+        <v>0.6376267297078108</v>
       </c>
       <c r="D74">
-        <v>1.26053619580922</v>
+        <v>4.095779762221372</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75">
-        <v>1.167736341502357</v>
+        <v>5.773887068071265</v>
       </c>
       <c r="B75">
-        <v>1.664280349470206</v>
+        <v>1.174177738296479</v>
       </c>
       <c r="C75">
-        <v>2.889999999999998</v>
+        <v>0.7493778359038915</v>
       </c>
       <c r="D75">
-        <v>1.957454020886822</v>
+        <v>1.323367899330259</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76">
-        <v>1.414649670867309</v>
+        <v>5.780619812056849</v>
       </c>
       <c r="B76">
-        <v>3.231118227487208</v>
+        <v>1.247323999999998</v>
       </c>
       <c r="C76">
-        <v>3.231118227487202</v>
+        <v>3.218193754577239</v>
       </c>
       <c r="D76">
-        <v>1.78673862592025</v>
+        <v>1.373762776524177</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77">
-        <v>1.759433804311464</v>
+        <v>1.41493012238093</v>
       </c>
       <c r="B77">
-        <v>2.890000000000011</v>
+        <v>1.414930122380923</v>
       </c>
       <c r="C77">
-        <v>4.08707719525826</v>
+        <v>5.934056078501479</v>
       </c>
       <c r="D77">
-        <v>7.706666666666558</v>
+        <v>1.949624204803274</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78">
-        <v>1.556312629261871</v>
+        <v>1.163065396136347</v>
       </c>
       <c r="B78">
-        <v>0.8811918593419483</v>
+        <v>1.657623228072316</v>
       </c>
       <c r="C78">
-        <v>0.695919732441472</v>
+        <v>2.035364443238608</v>
       </c>
       <c r="D78">
-        <v>2.619119007438751</v>
+        <v>1.779591671416566</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79">
-        <v>2.312</v>
+        <v>11.51376000000006</v>
       </c>
       <c r="B79">
-        <v>1.099635132946826</v>
+        <v>3.218193754577213</v>
       </c>
       <c r="C79">
-        <v>1.059666666666666</v>
+        <v>2.035364443238599</v>
       </c>
       <c r="D79">
-        <v>3.125229957092214</v>
+        <v>4.797399999999989</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80">
-        <v>5.780000000000022</v>
+        <v>1.408991072183835</v>
       </c>
       <c r="B80">
-        <v>1.157782576232327</v>
+        <v>2.87843999999999</v>
       </c>
       <c r="C80">
-        <v>1.651428571428573</v>
+        <v>3.865020463722507</v>
       </c>
       <c r="D80">
-        <v>2.409926139947033</v>
+        <v>4.070728886477234</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81">
-        <v>3.853333333333324</v>
+        <v>1.989046394316583</v>
       </c>
       <c r="B81">
-        <v>3.853333333333324</v>
+        <v>0.926967813902952</v>
       </c>
       <c r="C81">
-        <v>3.231118227487208</v>
+        <v>1.532917569276284</v>
       </c>
       <c r="D81">
-        <v>5.780000000000022</v>
+        <v>3.871663893820732</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82">
-        <v>1.131126549742285</v>
+        <v>2.022761446252237</v>
       </c>
       <c r="B82">
-        <v>5.780000000000022</v>
+        <v>1.061618600863846</v>
       </c>
       <c r="C82">
-        <v>4.308157636649611</v>
+        <v>2.967028039250715</v>
       </c>
       <c r="D82">
-        <v>3.853333333333324</v>
+        <v>4.06379753415453</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83">
-        <v>1.315576194001025</v>
+        <v>2.302751999999996</v>
       </c>
       <c r="B83">
-        <v>4.046000000000011</v>
+        <v>1.153151445927395</v>
       </c>
       <c r="C83">
-        <v>5.780000000000022</v>
+        <v>11.51376000000006</v>
       </c>
       <c r="D83">
-        <v>5.780000000000022</v>
+        <v>2.40028643538724</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84">
-        <v>1.140283595870934</v>
+        <v>6.436387509154529</v>
       </c>
       <c r="B84">
-        <v>2.246860130147072</v>
+        <v>3.837920000000021</v>
       </c>
       <c r="C84">
-        <v>1.438066620875303</v>
+        <v>3.218193754577213</v>
       </c>
       <c r="D84">
-        <v>1.262310890577344</v>
+        <v>5.756879999999929</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85">
-        <v>1.286286236197485</v>
+        <v>11.51376000000006</v>
       </c>
       <c r="B85">
-        <v>1.181273457708844</v>
+        <v>6.436387509154529</v>
       </c>
       <c r="C85">
-        <v>1.792838418731321</v>
+        <v>4.290925006102989</v>
       </c>
       <c r="D85">
-        <v>1.51387987102747</v>
+        <v>11.67257798514073</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86">
-        <v>1.167736341502354</v>
+        <v>3.837920000000021</v>
       </c>
       <c r="B86">
-        <v>1.203085434833207</v>
+        <v>4.029816000000014</v>
       </c>
       <c r="C86">
-        <v>1.6642803494702</v>
+        <v>6.436387509154529</v>
       </c>
       <c r="D86">
-        <v>1.35206788383572</v>
+        <v>12.13656867751306</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87">
-        <v>2.119333333333337</v>
+        <v>0.9684087417882877</v>
       </c>
       <c r="B87">
-        <v>1.204166666666668</v>
+        <v>2.237872689626456</v>
       </c>
       <c r="C87">
-        <v>2.030884986197024</v>
+        <v>1.410467494982359</v>
       </c>
       <c r="D87">
-        <v>1.570881113992305</v>
+        <v>6.436387509154347</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88">
-        <v>5.780000000000022</v>
+        <v>1.264739012808493</v>
       </c>
       <c r="B88">
-        <v>1.272864756282838</v>
+        <v>1.262148688205205</v>
       </c>
       <c r="C88">
-        <v>1.850502904618093</v>
+        <v>1.78566706505639</v>
       </c>
       <c r="D88">
-        <v>1.425630046143275</v>
+        <v>1.127060738529464</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89">
-        <v>5.780000000000022</v>
+        <v>1.23413315733289</v>
       </c>
       <c r="B89">
-        <v>1.537571942817259</v>
+        <v>1.198273093093875</v>
       </c>
       <c r="C89">
-        <v>5.77999999999997</v>
+        <v>1.632731371029344</v>
       </c>
       <c r="D89">
-        <v>5.780000000000022</v>
+        <v>1.470856761983118</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90">
-        <v>3.744766883578433</v>
+        <v>1.281141091252695</v>
       </c>
       <c r="B90">
-        <v>3.853333333333324</v>
+        <v>1.199350000000001</v>
       </c>
       <c r="C90">
-        <v>5.780000000000022</v>
+        <v>2.02276144625224</v>
       </c>
       <c r="D90">
-        <v>5.780000000000022</v>
+        <v>1.401741764567726</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91">
-        <v>1.284444444444441</v>
+        <v>1.163065396136347</v>
       </c>
       <c r="B91">
-        <v>3.231118227487208</v>
+        <v>1.233358028107908</v>
       </c>
       <c r="C91">
-        <v>2.889999999999985</v>
+        <v>2.035364443238608</v>
       </c>
       <c r="D91">
-        <v>4.112228676929076</v>
+        <v>1.564597589536338</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92">
-        <v>2.724718130172157</v>
+        <v>2.110855999999997</v>
       </c>
       <c r="B92">
-        <v>4.08707719525826</v>
+        <v>1.056743304137876</v>
       </c>
       <c r="C92">
-        <v>2.889999999999998</v>
+        <v>8.635320000000021</v>
       </c>
       <c r="D92">
-        <v>1.669777777777741</v>
+        <v>1.480265049628076</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93">
-        <v>0.8272585301020717</v>
+        <v>6.436387509154529</v>
       </c>
       <c r="B93">
-        <v>5.779999999999919</v>
+        <v>4.797400000000026</v>
       </c>
       <c r="C93">
-        <v>5.77999999999997</v>
+        <v>6.436387509154529</v>
       </c>
       <c r="D93">
-        <v>4.891018727988131</v>
+        <v>5.756879999999979</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94">
-        <v>1.007912735127727</v>
+        <v>5.756879999999979</v>
       </c>
       <c r="B94">
-        <v>3.473347728696953</v>
+        <v>3.218193754577265</v>
       </c>
       <c r="C94">
-        <v>3.853333333333324</v>
+        <v>5.934056078501481</v>
       </c>
       <c r="D94">
-        <v>0.9181646184956884</v>
+        <v>16.28291554590951</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95">
-        <v>1.046065707471908</v>
+        <v>3.729787816044103</v>
       </c>
       <c r="B95">
-        <v>1.388786983573177</v>
+        <v>6.068284338756746</v>
       </c>
       <c r="C95">
-        <v>1.041525786175769</v>
+        <v>2.878440000000003</v>
       </c>
       <c r="D95">
-        <v>1.117598133839505</v>
+        <v>11.67257798514127</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96">
-        <v>1.058890040855258</v>
+        <v>1.279306666666674</v>
       </c>
       <c r="B96">
-        <v>1.180782477964111</v>
+        <v>8.141457772954467</v>
       </c>
       <c r="C96">
-        <v>1.26036111111111</v>
+        <v>5.427638515302978</v>
       </c>
       <c r="D96">
-        <v>1.189699589030102</v>
+        <v>5.363656257628699</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97">
-        <v>1.058890040855258</v>
+        <v>2.713819257651489</v>
       </c>
       <c r="B97">
-        <v>1.222754681997039</v>
+        <v>8.635320000000046</v>
       </c>
       <c r="C97">
-        <v>1.386746656837301</v>
+        <v>6.396533333333368</v>
       </c>
       <c r="D97">
-        <v>1.262243072429953</v>
+        <v>4.058271486908613</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98">
-        <v>1.097182907100112</v>
+        <v>0.8239494959816629</v>
       </c>
       <c r="B98">
-        <v>1.324545335042251</v>
+        <v>3.459454337782194</v>
       </c>
       <c r="C98">
-        <v>1.568193050757606</v>
+        <v>0.9253940637869875</v>
       </c>
       <c r="D98">
-        <v>1.289678350008729</v>
+        <v>4.871454653076256</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99">
-        <v>1.420612572671612</v>
+        <v>0.9891072681443299</v>
       </c>
       <c r="B99">
-        <v>1.35623191158123</v>
+        <v>1.383231835638882</v>
       </c>
       <c r="C99">
-        <v>1.677555869246817</v>
+        <v>1.175798057804192</v>
       </c>
       <c r="D99">
-        <v>1.420612572671612</v>
+        <v>0.8713271894841559</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100">
-        <v>1.568193050757607</v>
+        <v>1.041881444642021</v>
       </c>
       <c r="B100">
-        <v>1.615559113743603</v>
+        <v>1.176059348052255</v>
       </c>
       <c r="C100">
-        <v>2.154078818324794</v>
+        <v>1.381199670209951</v>
       </c>
       <c r="D100">
-        <v>2.154078818324795</v>
+        <v>1.074095806196103</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101">
-        <v>1.634830878103298</v>
+        <v>1.054654480691837</v>
       </c>
       <c r="B101">
-        <v>2.043538597629121</v>
+        <v>1.21786366326905</v>
       </c>
       <c r="C101">
-        <v>1.651428571428569</v>
+        <v>1.492600591708309</v>
       </c>
       <c r="D101">
-        <v>3.0604563607254</v>
+        <v>1.184940790673982</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102">
-        <v>4.08707719525826</v>
+        <v>1.054654480691837</v>
       </c>
       <c r="B102">
-        <v>2.624727337396976</v>
+        <v>1.319247153702082</v>
       </c>
       <c r="C102">
-        <v>2.265959829321277</v>
+        <v>1.67084564576983</v>
       </c>
       <c r="D102">
-        <v>3.994069064892595</v>
+        <v>1.234168988525239</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103">
-        <v>5.780000000000022</v>
+        <v>1.092794175471709</v>
       </c>
       <c r="B103">
-        <v>1.322416493664552</v>
+        <v>1.224813189237982</v>
       </c>
       <c r="C103">
-        <v>3.046327479295596</v>
+        <v>2.237872689626468</v>
       </c>
       <c r="D103">
-        <v>7.706666666666741</v>
+        <v>1.289539168414868</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104">
-        <v>5.780000000000022</v>
+        <v>1.414930122380923</v>
       </c>
       <c r="B104">
-        <v>5.780000000000022</v>
+        <v>1.609096877288619</v>
       </c>
       <c r="C104">
-        <v>5.779999999999919</v>
+        <v>5.815326980681761</v>
       </c>
       <c r="D104">
-        <v>5.780000000000022</v>
+        <v>1.452613112682431</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105">
-        <v>5.780000000000022</v>
+        <v>1.561920278554572</v>
       </c>
       <c r="B105">
-        <v>4.334999999999964</v>
+        <v>1.843100892999616</v>
       </c>
       <c r="C105">
-        <v>3.162577671910091</v>
+        <v>4.408624744906758</v>
       </c>
       <c r="D105">
-        <v>5.780000000000022</v>
+        <v>2.145462503051497</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106">
-        <v>3.853333333333324</v>
+        <v>1.628291554590882</v>
       </c>
       <c r="B106">
-        <v>5.780000000000022</v>
+        <v>3.02664236186718</v>
       </c>
       <c r="C106">
-        <v>2.408333333333325</v>
+        <v>3.034142169378371</v>
       </c>
       <c r="D106">
-        <v>4.623999999999935</v>
+        <v>3.048214535282479</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107">
-        <v>0.8260596769296438</v>
+        <v>4.070728886477234</v>
       </c>
       <c r="B107">
-        <v>5.779999999999919</v>
+        <v>1.357757432487849</v>
       </c>
       <c r="C107">
-        <v>3.231118227487202</v>
+        <v>6.436387509154529</v>
       </c>
       <c r="D107">
-        <v>7.706666666666558</v>
+        <v>3.978092788633231</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108">
-        <v>0.9153426974953293</v>
+        <v>7.196100000000039</v>
       </c>
       <c r="B108">
-        <v>5.779999999999919</v>
+        <v>6.436387509154529</v>
       </c>
       <c r="C108">
-        <v>2.889999999999985</v>
+        <v>4.403427857397028</v>
       </c>
       <c r="D108">
-        <v>0.8511730867505654</v>
+        <v>23.02751999999931</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109">
-        <v>0.9937921995854018</v>
+        <v>6.918908675564385</v>
       </c>
       <c r="B109">
-        <v>1.388786983573177</v>
+        <v>4.797400000000025</v>
       </c>
       <c r="C109">
-        <v>3.473347728696983</v>
+        <v>4.965045045855752</v>
       </c>
       <c r="D109">
-        <v>0.9637528021928495</v>
+        <v>8.197800713557401</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110">
-        <v>1.077039409162399</v>
+        <v>5.756879999999929</v>
       </c>
       <c r="B110">
-        <v>1.180782477964113</v>
+        <v>8.635320000000046</v>
       </c>
       <c r="C110">
-        <v>0.879297240574489</v>
+        <v>5.166957929149317</v>
       </c>
       <c r="D110">
-        <v>1.092322745223938</v>
+        <v>1.91896000000001</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111">
-        <v>1.029449258115374</v>
+        <v>3.837920000000021</v>
       </c>
       <c r="B111">
-        <v>1.180782477964113</v>
+        <v>11.51376000000006</v>
       </c>
       <c r="C111">
-        <v>1.021769298814563</v>
+        <v>2.878440000000015</v>
       </c>
       <c r="D111">
-        <v>1.250412854038813</v>
+        <v>9.215504464997931</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112">
-        <v>1.06338470627412</v>
+        <v>0.8227554382219265</v>
       </c>
       <c r="B112">
-        <v>1.009175713118422</v>
+        <v>6.436387509154529</v>
       </c>
       <c r="C112">
-        <v>1.22909777997905</v>
+        <v>5.465200475704745</v>
       </c>
       <c r="D112">
-        <v>1.215634920634921</v>
+        <v>4.02981600000003</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113">
-        <v>1.445000000000002</v>
+        <v>0.9116813267053466</v>
       </c>
       <c r="B113">
-        <v>0.9765296934656834</v>
+        <v>6.436387509154347</v>
       </c>
       <c r="C113">
-        <v>1.49790675343137</v>
+        <v>0.8477543950011861</v>
       </c>
       <c r="D113">
-        <v>1.288117226288871</v>
+        <v>10.93040095140952</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114">
-        <v>1.204166666666667</v>
+        <v>0.9898170307870591</v>
       </c>
       <c r="B114">
-        <v>1.260858133107934</v>
+        <v>1.383231835638882</v>
       </c>
       <c r="C114">
-        <v>1.533147290629451</v>
+        <v>0.9898170307870608</v>
       </c>
       <c r="D114">
-        <v>1.651428571428573</v>
+        <v>0.8346785148735839</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115">
-        <v>1.257394029798721</v>
+        <v>1.07273125152575</v>
       </c>
       <c r="B115">
-        <v>1.284444444444447</v>
+        <v>1.176059348052255</v>
       </c>
       <c r="C115">
-        <v>1.752805475378687</v>
+        <v>1.224181388859136</v>
       </c>
       <c r="D115">
-        <v>2.075083505682501</v>
+        <v>0.9462967576015583</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116">
-        <v>1.450755431489217</v>
+        <v>1.025331461082913</v>
       </c>
       <c r="B116">
-        <v>2.246860130147054</v>
+        <v>1.176059348052255</v>
       </c>
       <c r="C116">
-        <v>1.926666666666668</v>
+        <v>1.491915126417644</v>
       </c>
       <c r="D116">
-        <v>2.264659315230206</v>
+        <v>1.087953454243042</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117">
-        <v>1.634830878103298</v>
+        <v>1.059131167449022</v>
       </c>
       <c r="B117">
-        <v>2.41266443884028</v>
+        <v>0.9828853906537089</v>
       </c>
       <c r="C117">
-        <v>1.651428571428573</v>
+        <v>1.414339854897734</v>
       </c>
       <c r="D117">
-        <v>2.5690936709761</v>
+        <v>1.245411202622659</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118">
-        <v>2.194859628797123</v>
+        <v>1.439219999999998</v>
       </c>
       <c r="B118">
-        <v>3.046327479295523</v>
+        <v>1.070557098604298</v>
       </c>
       <c r="C118">
-        <v>1.651428571428571</v>
+        <v>1.745794253477173</v>
       </c>
       <c r="D118">
-        <v>3.518867608622883</v>
+        <v>1.185514093441588</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119">
-        <v>2.408333333333325</v>
+        <v>1.19935</v>
       </c>
       <c r="B119">
-        <v>2.283729941224304</v>
+        <v>1.31975604104941</v>
       </c>
       <c r="C119">
-        <v>1.651428571428573</v>
+        <v>1.918959999999999</v>
       </c>
       <c r="D119">
-        <v>2.898685550490162</v>
+        <v>1.282964757383714</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120">
-        <v>5.780000000000022</v>
+        <v>1.25236445367953</v>
       </c>
       <c r="B120">
-        <v>1.504774770891346</v>
+        <v>1.439219999999998</v>
       </c>
       <c r="C120">
-        <v>2.265959829321323</v>
+        <v>1.644822857142858</v>
       </c>
       <c r="D120">
-        <v>3.046327479295499</v>
+        <v>1.644822857142858</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121">
-        <v>3.853333333333324</v>
+        <v>1.516451745580009</v>
       </c>
       <c r="B121">
-        <v>2.011499054050095</v>
+        <v>2.145462503051498</v>
       </c>
       <c r="C121">
-        <v>2.204027489440896</v>
+        <v>3.991497049466804</v>
       </c>
       <c r="D121">
-        <v>7.706666666666741</v>
+        <v>2.066783171659765</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122">
-        <v>0.8047021379766521</v>
+        <v>1.628291554590882</v>
       </c>
       <c r="B122">
-        <v>3.473347728696983</v>
+        <v>2.335450970306186</v>
       </c>
       <c r="C122">
-        <v>1.284444444444442</v>
+        <v>3.991497049466804</v>
       </c>
       <c r="D122">
-        <v>0.8047021379766521</v>
+        <v>2.255600677969293</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123">
-        <v>0.8858244468388098</v>
+        <v>2.186080190281942</v>
       </c>
       <c r="B123">
-        <v>3.47334772869694</v>
+        <v>2.593785051482985</v>
       </c>
       <c r="C123">
-        <v>3.473347728696953</v>
+        <v>4.40862474490677</v>
       </c>
       <c r="D123">
-        <v>0.913583913989971</v>
+        <v>2.739520377916554</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124">
-        <v>1.11742101032409</v>
+        <v>2.398700000000013</v>
       </c>
       <c r="B124">
-        <v>2.937380206806552</v>
+        <v>2.320672519301253</v>
       </c>
       <c r="C124">
-        <v>2.408333333333351</v>
+        <v>2.195211379483166</v>
       </c>
       <c r="D124">
-        <v>1.186537236464894</v>
+        <v>3.504792138188446</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125">
-        <v>1.363210273582179</v>
+        <v>6.436387509154529</v>
       </c>
       <c r="B125">
-        <v>5.780000000000022</v>
+        <v>2.237872689626447</v>
       </c>
       <c r="C125">
-        <v>5.780000000000022</v>
+        <v>1.279306666666668</v>
       </c>
       <c r="D125">
-        <v>2.437061983436431</v>
+        <v>2.887090808288169</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126">
-        <v>1.260361111111112</v>
+        <v>8.581850012206038</v>
       </c>
       <c r="B126">
-        <v>1.068183707472929</v>
+        <v>2.003453057833909</v>
       </c>
       <c r="C126">
-        <v>0.8047021379766521</v>
+        <v>3.459454337782194</v>
       </c>
       <c r="D126">
-        <v>2.246989196989809</v>
+        <v>3.034142169378371</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127">
-        <v>1.329415512523557</v>
+        <v>8.141457772954324</v>
       </c>
       <c r="B127">
-        <v>1.046065707471908</v>
+        <v>3.459454337782207</v>
       </c>
       <c r="C127">
-        <v>0.9456435998309487</v>
+        <v>2.398699999999987</v>
       </c>
       <c r="D127">
-        <v>2.267375750928609</v>
+        <v>11.51375999999965</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128">
-        <v>1.432097955991682</v>
+        <v>11.51375999999965</v>
       </c>
       <c r="B128">
-        <v>1.388786983573176</v>
+        <v>3.198266666666684</v>
       </c>
       <c r="C128">
-        <v>1.26721755843896</v>
+        <v>11.51375999999986</v>
       </c>
       <c r="D128">
-        <v>2.55642887243408</v>
+        <v>4.612605783709446</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129">
-        <v>1.568193050757605</v>
+        <v>3.837920000000021</v>
       </c>
       <c r="B129">
-        <v>1.970404898708027</v>
+        <v>8.141457772954467</v>
       </c>
       <c r="C129">
-        <v>1.651428571428573</v>
+        <v>8.581850012205857</v>
       </c>
       <c r="D129">
-        <v>2.750522467787738</v>
+        <v>23.02751999999931</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130">
-        <v>1.740010416635489</v>
+        <v>0.8014833294247481</v>
       </c>
       <c r="B130">
-        <v>1.820853943749226</v>
+        <v>11.51376000000006</v>
       </c>
       <c r="C130">
-        <v>1.651428571428573</v>
+        <v>4.317659999999922</v>
       </c>
       <c r="D130">
-        <v>3.243012012571398</v>
+        <v>16.28291554590836</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131">
-        <v>2.154078818324797</v>
+        <v>0.8822811490514562</v>
       </c>
       <c r="B131">
-        <v>3.04632747929555</v>
+        <v>3.981916040633945</v>
       </c>
       <c r="C131">
-        <v>1.651428571428571</v>
+        <v>8.14145777295418</v>
       </c>
       <c r="D131">
-        <v>3.916506942408704</v>
+        <v>1.016964290556643E-13</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132">
-        <v>2.724718130172157</v>
+        <v>1.112951326282792</v>
       </c>
       <c r="B132">
-        <v>2.593854382103109</v>
+        <v>6.436387509154325</v>
       </c>
       <c r="C132">
-        <v>1.548214285714286</v>
+        <v>0.8115249287190317</v>
       </c>
       <c r="D132">
-        <v>4.816666666666703</v>
+        <v>16.28291554590836</v>
       </c>
     </row>
     <row r="133" spans="1:4">
       <c r="A133">
-        <v>2.724718130172157</v>
+        <v>1.357757432487853</v>
       </c>
       <c r="B133">
-        <v>2.808575162683808</v>
+        <v>1.063910972643039</v>
       </c>
       <c r="C133">
-        <v>1.548214285714284</v>
+        <v>0.9251942100724626</v>
       </c>
       <c r="D133">
-        <v>5.780000000000022</v>
+        <v>0.8052596014018228</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134">
-        <v>0.7661088651044407</v>
+        <v>1.255319666666667</v>
       </c>
       <c r="B134">
-        <v>1.897474747474742</v>
+        <v>1.04188144464202</v>
       </c>
       <c r="C134">
-        <v>2.219040465960243</v>
+        <v>1.262148688205205</v>
       </c>
       <c r="D134">
-        <v>0.7619286292639617</v>
+        <v>0.9008336169482342</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135">
-        <v>0.7755958431903752</v>
+        <v>1.28387561904762</v>
       </c>
       <c r="B135">
-        <v>1.868059407378958</v>
+        <v>1.383231835638882</v>
       </c>
       <c r="C135">
-        <v>1.651428571428573</v>
+        <v>5.815326980681761</v>
       </c>
       <c r="D135">
-        <v>0.7808138481371888</v>
+        <v>1.181791087519034</v>
       </c>
     </row>
     <row r="136" spans="1:4">
       <c r="A136">
-        <v>0.9787270104434111</v>
+        <v>1.444952409763263</v>
       </c>
       <c r="B136">
-        <v>1.997034532446364</v>
+        <v>1.496811393550045</v>
       </c>
       <c r="C136">
-        <v>0.7581686897760385</v>
+        <v>1.644822857142858</v>
       </c>
       <c r="D136">
-        <v>1.032876488398099</v>
+        <v>2.066783171659775</v>
       </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137">
-        <v>1.614840927838473</v>
+        <v>1.628291554590888</v>
       </c>
       <c r="B137">
-        <v>0.3515172558859566</v>
+        <v>2.015653813378615</v>
       </c>
       <c r="C137">
-        <v>0.7894963442100514</v>
+        <v>1.644822857142858</v>
       </c>
       <c r="D137">
-        <v>2.872105091099727</v>
+        <v>2.238001240201851</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138">
-        <v>1.363210273582179</v>
+        <v>1.733050374968941</v>
       </c>
       <c r="B138">
-        <v>1.434898228567236</v>
+        <v>3.013171269510596</v>
       </c>
       <c r="C138">
-        <v>1.09732109724089</v>
+        <v>1.54202142857143</v>
       </c>
       <c r="D138">
-        <v>2.437061983436431</v>
+        <v>2.247258457382988</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139">
-        <v>1.31230153282959</v>
+        <v>2.145462503051498</v>
       </c>
       <c r="B139">
-        <v>0.890995448046241</v>
+        <v>2.145462503051497</v>
       </c>
       <c r="C139">
-        <v>1.651428571428573</v>
+        <v>3.973215737665501</v>
       </c>
       <c r="D139">
-        <v>2.255105516131979</v>
+        <v>2.277081878011717</v>
       </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140">
-        <v>1.461680144835042</v>
+        <v>11.51375999999965</v>
       </c>
       <c r="B140">
-        <v>1.269818285952302</v>
+        <v>2.620627778450044</v>
       </c>
       <c r="C140">
-        <v>1.651428571428573</v>
+        <v>2.210164304096436</v>
       </c>
       <c r="D140">
-        <v>2.547328859583932</v>
+        <v>2.749970147876167</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141">
-        <v>1.568193050757602</v>
+        <v>2.713819257651489</v>
       </c>
       <c r="B141">
-        <v>0.5504761904761911</v>
+        <v>2.56041172630791</v>
       </c>
       <c r="C141">
-        <v>1.548214285714286</v>
+        <v>1.644822857142858</v>
       </c>
       <c r="D141">
-        <v>2.31291422588582</v>
+        <v>3.230039964521081</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142">
-        <v>1.634830878103298</v>
+        <v>2.713819257651489</v>
       </c>
       <c r="B142">
-        <v>2.301586000700923</v>
+        <v>1.87667243293753</v>
       </c>
       <c r="C142">
-        <v>1.548214285714286</v>
+        <v>11.51376000000006</v>
       </c>
       <c r="D142">
-        <v>2.203452432278759</v>
+        <v>3.900840914639074</v>
       </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143">
-        <v>1.839184737866214</v>
+        <v>0.763044429644022</v>
       </c>
       <c r="B143">
-        <v>2.362254603657282</v>
+        <v>1.989046394316593</v>
       </c>
       <c r="C143">
-        <v>1.651428571428569</v>
+        <v>8.141457772954467</v>
       </c>
       <c r="D143">
-        <v>2.808575162683827</v>
+        <v>5.465200475704647</v>
       </c>
     </row>
     <row r="144" spans="1:4">
       <c r="A144">
-        <v>1.736673864348494</v>
+        <v>0.7724934598176155</v>
       </c>
       <c r="B144">
-        <v>2.198849219225573</v>
+        <v>0.3501111868624127</v>
       </c>
       <c r="C144">
-        <v>2.219040465960243</v>
+        <v>8.581850012205917</v>
       </c>
       <c r="D144">
-        <v>2.015825470255479</v>
+        <v>4.290925006103141</v>
       </c>
     </row>
     <row r="145" spans="1:4">
       <c r="A145">
-        <v>3.853333333333324</v>
+        <v>0.9748121024016378</v>
       </c>
       <c r="B145">
-        <v>2.198849219225564</v>
+        <v>1.429158635652962</v>
       </c>
       <c r="C145">
-        <v>1.789047619047623</v>
+        <v>0.7822987947681684</v>
       </c>
       <c r="D145">
-        <v>7.706666666666741</v>
+        <v>0.7717913933407896</v>
       </c>
     </row>
     <row r="146" spans="1:4">
       <c r="A146">
-        <v>3.853333333333324</v>
+        <v>1.60838156412712</v>
       </c>
       <c r="B146">
-        <v>2.467337206157437</v>
+        <v>0.8874314662540568</v>
       </c>
       <c r="C146">
-        <v>1.926666666666674</v>
+        <v>0.7863383588332122</v>
       </c>
       <c r="D146">
-        <v>7.706666666666741</v>
+        <v>0.7776905927446415</v>
       </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147">
-        <v>3.853333333333324</v>
+        <v>1.357757432487851</v>
       </c>
       <c r="B147">
-        <v>2.267803654037368</v>
+        <v>1.264739012808491</v>
       </c>
       <c r="C147">
-        <v>1.541333333333337</v>
+        <v>1.092931812851928</v>
       </c>
       <c r="D147">
-        <v>7.706666666666741</v>
+        <v>1.028744982444507</v>
       </c>
     </row>
     <row r="148" spans="1:4">
       <c r="A148">
-        <v>1.541333333333337</v>
+        <v>1.307052326698273</v>
       </c>
       <c r="B148">
-        <v>2.408333333333333</v>
+        <v>0.5482742857142859</v>
       </c>
       <c r="C148">
-        <v>1.445000000000002</v>
+        <v>5.80168129825315</v>
       </c>
       <c r="D148">
-        <v>1.541333333333337</v>
+        <v>2.855068846264214</v>
       </c>
     </row>
     <row r="149" spans="1:4">
       <c r="A149">
-        <v>1.284444444444447</v>
+        <v>1.381199670209951</v>
       </c>
       <c r="B149">
-        <v>3.473347728696983</v>
+        <v>2.068058268797899</v>
       </c>
       <c r="C149">
-        <v>1.445000000000001</v>
+        <v>3.973215737665501</v>
       </c>
       <c r="D149">
-        <v>1.360000000000003</v>
+        <v>2.238001240201847</v>
       </c>
     </row>
     <row r="150" spans="1:4">
       <c r="A150">
-        <v>1.468644591436879</v>
+        <v>1.670845645769831</v>
       </c>
       <c r="B150">
-        <v>2.929863952093653</v>
+        <v>2.352805585242645</v>
       </c>
       <c r="C150">
-        <v>1.548214285714286</v>
+        <v>1.644822857142858</v>
       </c>
       <c r="D150">
-        <v>2.508350256033726</v>
+        <v>2.255600677969289</v>
       </c>
     </row>
     <row r="151" spans="1:4">
       <c r="A151">
-        <v>1.487718555372621</v>
+        <v>1.628291554590888</v>
       </c>
       <c r="B151">
-        <v>2.889999999999998</v>
+        <v>2.190053822348665</v>
       </c>
       <c r="C151">
-        <v>1.651428571428571</v>
+        <v>1.54202142857143</v>
       </c>
       <c r="D151">
-        <v>2.429553595542011</v>
+        <v>2.265408045050802</v>
       </c>
     </row>
     <row r="152" spans="1:4">
       <c r="A152">
-        <v>1.391250469406012</v>
+        <v>1.83182799891474</v>
       </c>
       <c r="B152">
-        <v>1.284444444444444</v>
+        <v>2.190053822348664</v>
       </c>
       <c r="C152">
-        <v>1.651428571428573</v>
+        <v>3.973215737665501</v>
       </c>
       <c r="D152">
-        <v>2.264659315230207</v>
+        <v>2.469099236423708</v>
       </c>
     </row>
     <row r="153" spans="1:4">
       <c r="A153">
-        <v>1.461680144835043</v>
+        <v>1.72972716889109</v>
       </c>
       <c r="B153">
-        <v>1.685623068898034</v>
+        <v>2.660719523620642</v>
       </c>
       <c r="C153">
-        <v>1.78904761904762</v>
+        <v>1.644822857142858</v>
       </c>
       <c r="D153">
-        <v>2.108863101250192</v>
+        <v>2.494647999999997</v>
       </c>
     </row>
     <row r="154" spans="1:4">
       <c r="A154">
-        <v>1.568193050757601</v>
+        <v>3.837920000000021</v>
       </c>
       <c r="B154">
-        <v>2.191583333333338</v>
+        <v>2.25873243942122</v>
       </c>
       <c r="C154">
-        <v>2.204027489440896</v>
+        <v>1.781891428571428</v>
       </c>
       <c r="D154">
-        <v>2.157099931312942</v>
+        <v>2.797340862033066</v>
       </c>
     </row>
     <row r="155" spans="1:4">
       <c r="A155">
-        <v>1.740010416635482</v>
+        <v>3.837920000000021</v>
       </c>
       <c r="B155">
-        <v>1.618428670380969</v>
+        <v>2.398700000000013</v>
       </c>
       <c r="C155">
-        <v>1.756973104826499</v>
+        <v>5.836288992570566</v>
       </c>
       <c r="D155">
-        <v>2.456943668822945</v>
+        <v>2.007762168374429</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156">
-        <v>1.926666666666665</v>
+        <v>3.837920000000021</v>
       </c>
       <c r="B156">
-        <v>1.941660407715233</v>
+        <v>3.459454337782207</v>
       </c>
       <c r="C156">
-        <v>2.006366361188463</v>
+        <v>11.51376000000006</v>
       </c>
       <c r="D156">
-        <v>2.1949483118827</v>
+        <v>7.67583999999995</v>
       </c>
     </row>
     <row r="157" spans="1:4">
       <c r="A157">
-        <v>2.408333333333339</v>
+        <v>1.535167999999999</v>
       </c>
       <c r="B157">
-        <v>1.941660407715225</v>
+        <v>2.918144496285283</v>
       </c>
       <c r="C157">
-        <v>2.312</v>
+        <v>1.535167999999999</v>
       </c>
       <c r="D157">
-        <v>2.299720935944175</v>
+        <v>12.13656867751386</v>
       </c>
     </row>
     <row r="158" spans="1:4">
       <c r="A158">
-        <v>3.85333333333337</v>
+        <v>1.279306666666666</v>
       </c>
       <c r="B158">
-        <v>2.412664438840256</v>
+        <v>11.51375999999965</v>
       </c>
       <c r="C158">
-        <v>1.037541752841251</v>
+        <v>1.439219999999998</v>
       </c>
       <c r="D158">
-        <v>2.890000000000011</v>
+        <v>7.67583999999995</v>
       </c>
     </row>
     <row r="159" spans="1:4">
       <c r="A159">
-        <v>1.060987253150482</v>
+        <v>1.462770013071129</v>
       </c>
       <c r="B159">
-        <v>2.859331720680346</v>
+        <v>2.878440000000003</v>
       </c>
       <c r="C159">
-        <v>0.7706666666666667</v>
+        <v>3.973215737665435</v>
       </c>
       <c r="D159">
-        <v>1.048075441711751</v>
+        <v>1.535167999999999</v>
       </c>
     </row>
     <row r="160" spans="1:4">
       <c r="A160">
-        <v>0.88923076923077</v>
+        <v>1.481767681151131</v>
       </c>
       <c r="B160">
-        <v>1.614840927838474</v>
+        <v>1.439219999999998</v>
       </c>
       <c r="C160">
-        <v>0.8670000000000004</v>
+        <v>3.973215737665501</v>
       </c>
       <c r="D160">
-        <v>0.8257142857142861</v>
+        <v>1.354559999999999</v>
       </c>
     </row>
     <row r="161" spans="1:4">
       <c r="A161">
-        <v>0.92628205128205</v>
+        <v>1.385685467528388</v>
       </c>
       <c r="B161">
-        <v>2.312</v>
+        <v>1.481767681151131</v>
       </c>
       <c r="C161">
-        <v>0.963333333333334</v>
+        <v>3.973215737665501</v>
       </c>
       <c r="D161">
-        <v>0.8945238095238091</v>
+        <v>2.413415581313749</v>
       </c>
     </row>
     <row r="162" spans="1:4">
       <c r="A162">
-        <v>1.007121212121212</v>
+        <v>1.414930122380927</v>
       </c>
       <c r="B162">
-        <v>1.480249082309799</v>
+        <v>1.847647355326056</v>
       </c>
       <c r="C162">
-        <v>0.963333333333334</v>
+        <v>3.991497049466804</v>
       </c>
       <c r="D162">
-        <v>0.9842753623188409</v>
+        <v>2.51131403619878</v>
       </c>
     </row>
     <row r="163" spans="1:4">
       <c r="A163">
-        <v>1.050909090909093</v>
+        <v>1.648388486424089</v>
       </c>
       <c r="B163">
-        <v>1.059666666666666</v>
+        <v>1.572126322726035</v>
       </c>
       <c r="C163">
-        <v>1.651428571428569</v>
+        <v>5.808280714285745</v>
       </c>
       <c r="D163">
-        <v>1.005217391304349</v>
+        <v>2.247258457382994</v>
       </c>
     </row>
     <row r="164" spans="1:4">
       <c r="A164">
-        <v>1.615559113743603</v>
+        <v>1.831827998914746</v>
       </c>
       <c r="B164">
-        <v>1.103454545454547</v>
+        <v>1.933893766084378</v>
       </c>
       <c r="C164">
-        <v>1.651428571428571</v>
+        <v>2.176975161372471</v>
       </c>
       <c r="D164">
-        <v>2.990990991479442</v>
+        <v>2.265408045050807</v>
       </c>
     </row>
     <row r="165" spans="1:4">
       <c r="A165">
-        <v>1.639288525129864</v>
+        <v>1.918959999999999</v>
       </c>
       <c r="B165">
-        <v>1.103454545454547</v>
+        <v>1.933893766084375</v>
       </c>
       <c r="C165">
-        <v>1.651428571428571</v>
+        <v>2.326776849997218</v>
       </c>
       <c r="D165">
-        <v>2.445905156845045</v>
+        <v>2.165553296271107</v>
       </c>
     </row>
     <row r="166" spans="1:4">
       <c r="A166">
-        <v>1.540488341933379</v>
+        <v>2.398699999999995</v>
       </c>
       <c r="B166">
-        <v>1.156</v>
+        <v>2.403013781084917</v>
       </c>
       <c r="C166">
-        <v>1.651428571428571</v>
+        <v>4.006906115667817</v>
       </c>
       <c r="D166">
-        <v>2.274506069328113</v>
+        <v>2.318688190148908</v>
       </c>
     </row>
     <row r="167" spans="1:4">
       <c r="A167">
-        <v>1.578440083058268</v>
+        <v>3.837920000000021</v>
       </c>
       <c r="B167">
-        <v>1.363210273582179</v>
+        <v>2.847894393797623</v>
       </c>
       <c r="C167">
-        <v>1.651428571428573</v>
+        <v>2.302751999999996</v>
       </c>
       <c r="D167">
-        <v>2.286226785152313</v>
+        <v>2.309605428571426</v>
       </c>
     </row>
     <row r="168" spans="1:4">
       <c r="A168">
-        <v>1.618428670380974</v>
+        <v>1.056743304137876</v>
       </c>
       <c r="B168">
-        <v>1.549777002327897</v>
+        <v>1.608381564127114</v>
       </c>
       <c r="C168">
-        <v>2.265959829321293</v>
+        <v>1.033391585829882</v>
       </c>
       <c r="D168">
-        <v>2.298326595313331</v>
+        <v>2.290522052200395</v>
       </c>
     </row>
     <row r="169" spans="1:4">
       <c r="A169">
-        <v>1.772376261156499</v>
+        <v>0.885673846153846</v>
       </c>
       <c r="B169">
-        <v>1.782100246969689</v>
+        <v>2.302751999999996</v>
       </c>
       <c r="C169">
-        <v>2.631152388002052</v>
+        <v>0.7675839999999996</v>
       </c>
       <c r="D169">
-        <v>2.490358526838838</v>
+        <v>2.878440000000015</v>
       </c>
     </row>
     <row r="170" spans="1:4">
       <c r="A170">
-        <v>1.839184737866205</v>
+        <v>0.9225769230769227</v>
       </c>
       <c r="B170">
-        <v>1.908456673226505</v>
+        <v>11.51375999999965</v>
       </c>
       <c r="C170">
-        <v>2.246860130147052</v>
+        <v>0.863532</v>
       </c>
       <c r="D170">
-        <v>2.044106168421248</v>
+        <v>1.0438831399449</v>
       </c>
     </row>
     <row r="171" spans="1:4">
       <c r="A171">
-        <v>2.246860130147052</v>
+        <v>1.003092727272727</v>
       </c>
       <c r="B171">
-        <v>1.941660407715244</v>
+        <v>1.474328085980567</v>
       </c>
       <c r="C171">
-        <v>1.651428571428573</v>
+        <v>0.9594800000000009</v>
       </c>
       <c r="D171">
-        <v>2.246860130147033</v>
+        <v>0.8224114285714283</v>
       </c>
     </row>
     <row r="172" spans="1:4">
       <c r="A172">
-        <v>1.664280349470199</v>
+        <v>1.046705454545453</v>
       </c>
       <c r="B172">
-        <v>2.371933253932545</v>
+        <v>1.055428</v>
       </c>
       <c r="C172">
-        <v>1.651428571428573</v>
+        <v>0.9594800000000022</v>
       </c>
       <c r="D172">
-        <v>2.455025067414314</v>
+        <v>0.8909457142857142</v>
       </c>
     </row>
     <row r="173" spans="1:4">
       <c r="A173">
-        <v>1.6642803494702</v>
+        <v>1.609096877288625</v>
       </c>
       <c r="B173">
-        <v>2.102986674087336</v>
+        <v>1.099040727272727</v>
       </c>
       <c r="C173">
-        <v>2.219040465960273</v>
+        <v>5.801681298253048</v>
       </c>
       <c r="D173">
-        <v>2.455025067414314</v>
+        <v>0.9803382608695654</v>
       </c>
     </row>
     <row r="174" spans="1:4">
       <c r="A174">
-        <v>1.699469871990964</v>
+        <v>1.632731371029347</v>
       </c>
       <c r="B174">
-        <v>2.978943814508771</v>
+        <v>1.099040727272727</v>
       </c>
       <c r="C174">
-        <v>1.752805475378681</v>
+        <v>3.973215737665435</v>
       </c>
       <c r="D174">
-        <v>2.286226785152313</v>
+        <v>1.001196521739131</v>
       </c>
     </row>
     <row r="175" spans="1:4">
       <c r="A175">
-        <v>1.677555869246821</v>
+        <v>1.534326388565646</v>
       </c>
       <c r="B175">
-        <v>1.445000000000005</v>
+        <v>1.151375999999998</v>
       </c>
       <c r="C175">
-        <v>2.593854382103122</v>
+        <v>5.815326980681711</v>
       </c>
       <c r="D175">
-        <v>2.114189660183274</v>
+        <v>2.412572346190676</v>
       </c>
     </row>
     <row r="176" spans="1:4">
       <c r="A176">
-        <v>1.74001041663549</v>
+        <v>1.572126322726034</v>
       </c>
       <c r="B176">
-        <v>1.6642803494702</v>
+        <v>1.317126827689892</v>
       </c>
       <c r="C176">
-        <v>3.046327479295548</v>
+        <v>5.815326980681761</v>
       </c>
       <c r="D176">
-        <v>1.957454020886822</v>
+        <v>2.702895698461078</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177">
-        <v>1.850502904618088</v>
+        <v>1.535917410833018</v>
       </c>
       <c r="B177">
-        <v>2.096150883423496</v>
+        <v>1.646408534612369</v>
       </c>
       <c r="C177">
-        <v>3.112625258523753</v>
+        <v>5.815326980681761</v>
       </c>
       <c r="D177">
-        <v>2.194642194481796</v>
+        <v>2.2654080450508</v>
       </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178">
-        <v>3.231118227487202</v>
+        <v>1.765286756111874</v>
       </c>
       <c r="B178">
-        <v>2.124198034611989</v>
+        <v>1.774971845981812</v>
       </c>
       <c r="C178">
-        <v>3.231118227487208</v>
+        <v>2.993622787100078</v>
       </c>
       <c r="D178">
-        <v>3.162577671910094</v>
+        <v>2.277081878011707</v>
       </c>
     </row>
     <row r="179" spans="1:4">
       <c r="A179">
-        <v>3.971925086011693</v>
+        <v>1.831827998914746</v>
       </c>
       <c r="B179">
-        <v>2.569093670976098</v>
+        <v>1.900822846533597</v>
       </c>
       <c r="C179">
-        <v>2.312</v>
+        <v>2.651887227933263</v>
       </c>
       <c r="D179">
-        <v>4.597611430318772</v>
+        <v>2.163389695581354</v>
       </c>
     </row>
     <row r="180" spans="1:4">
       <c r="A180">
-        <v>3.231118227487208</v>
+        <v>2.23787268962646</v>
       </c>
       <c r="B180">
-        <v>2.60420185891866</v>
+        <v>1.933893766084376</v>
       </c>
       <c r="C180">
-        <v>2.890000000000011</v>
+        <v>2.398700000000006</v>
       </c>
       <c r="D180">
-        <v>4.061769972394091</v>
+        <v>2.026982857268193</v>
       </c>
     </row>
     <row r="181" spans="1:4">
       <c r="A181">
-        <v>2.408333333333333</v>
+        <v>1.657623228072321</v>
       </c>
       <c r="B181">
-        <v>2.246860130147048</v>
+        <v>2.362445520916836</v>
       </c>
       <c r="C181">
-        <v>3.231118227487208</v>
+        <v>5.815326980681661</v>
       </c>
       <c r="D181">
-        <v>2.841225145343218</v>
+        <v>2.014454101831574</v>
       </c>
     </row>
     <row r="182" spans="1:4">
       <c r="A182">
-        <v>2.507957951485588</v>
+        <v>1.657623228072321</v>
       </c>
       <c r="B182">
-        <v>3.046327479295548</v>
+        <v>2.541377086743537</v>
       </c>
       <c r="C182">
-        <v>2.890000000000011</v>
+        <v>5.815326980681711</v>
       </c>
       <c r="D182">
-        <v>3.009549541782703</v>
+        <v>2.306302891854783</v>
       </c>
     </row>
     <row r="183" spans="1:4">
       <c r="A183">
-        <v>1.926666666666662</v>
+        <v>1.692671992503003</v>
       </c>
       <c r="B183">
-        <v>0.9633333333333256</v>
+        <v>2.96702803925074</v>
       </c>
       <c r="C183">
-        <v>0.6084210526315795</v>
+        <v>4.395287070652495</v>
       </c>
       <c r="D183">
-        <v>2.312</v>
+        <v>2.445204967144652</v>
       </c>
     </row>
     <row r="184" spans="1:4">
       <c r="A184">
-        <v>0.7706666666666667</v>
+        <v>1.670845645769832</v>
       </c>
       <c r="B184">
-        <v>3.473347728696996</v>
+        <v>1.439219999999995</v>
       </c>
       <c r="C184">
-        <v>0.8973558031807326</v>
+        <v>3.939976420259924</v>
       </c>
       <c r="D184">
-        <v>0.6800000000000004</v>
+        <v>2.445204967144652</v>
       </c>
     </row>
     <row r="185" spans="1:4">
       <c r="A185">
-        <v>1.091777777777773</v>
+        <v>1.628291554590885</v>
       </c>
       <c r="B185">
-        <v>1.926666666666674</v>
+        <v>1.657623228072321</v>
       </c>
       <c r="C185">
-        <v>1.1109235146039</v>
+        <v>2.583478964574695</v>
       </c>
       <c r="D185">
-        <v>0.9833968285282363</v>
+        <v>2.277081878011711</v>
       </c>
     </row>
     <row r="186" spans="1:4">
       <c r="A186">
-        <v>1.408503294587624</v>
+        <v>1.843100892999616</v>
       </c>
       <c r="B186">
-        <v>1.119903039030809</v>
+        <v>2.0877662798898</v>
       </c>
       <c r="C186">
-        <v>2.032309651518679</v>
+        <v>2.145462503051505</v>
       </c>
       <c r="D186">
-        <v>1.23753664475038</v>
+        <v>2.105732901542554</v>
       </c>
     </row>
     <row r="187" spans="1:4">
       <c r="A187">
-        <v>2.030884986197033</v>
+        <v>2.302752000000012</v>
       </c>
       <c r="B187">
-        <v>0.9213055926026635</v>
+        <v>2.11570124247354</v>
       </c>
       <c r="C187">
-        <v>2.062330066683913</v>
+        <v>3.100174757489618</v>
       </c>
       <c r="D187">
-        <v>2.031238459953201</v>
+        <v>1.863711993508833</v>
       </c>
     </row>
     <row r="188" spans="1:4">
       <c r="A188">
-        <v>1.514678081757974</v>
+        <v>3.218193754577219</v>
       </c>
       <c r="B188">
-        <v>1.454156749810922</v>
+        <v>2.558817296292192</v>
       </c>
       <c r="C188">
-        <v>2.091362370599074</v>
+        <v>5.836288992570531</v>
       </c>
       <c r="D188">
-        <v>1.719945972086986</v>
+        <v>1.949624204803286</v>
       </c>
     </row>
     <row r="189" spans="1:4">
       <c r="A189">
-        <v>1.3005</v>
+        <v>5.836288992570531</v>
       </c>
       <c r="B189">
-        <v>1.028932181082693</v>
+        <v>2.558817296292193</v>
       </c>
       <c r="C189">
-        <v>1.284444444444444</v>
+        <v>7.714123728762498</v>
       </c>
       <c r="D189">
-        <v>2.700805343161739</v>
+        <v>5.870888691482238</v>
       </c>
     </row>
     <row r="190" spans="1:4">
       <c r="A190">
-        <v>1.156</v>
+        <v>4.965045045855878</v>
       </c>
       <c r="B190">
-        <v>1.089887252068866</v>
+        <v>3.034142169378371</v>
       </c>
       <c r="C190">
-        <v>1.926666666666668</v>
+        <v>7.735575064337533</v>
       </c>
       <c r="D190">
-        <v>1.216842105263159</v>
+        <v>6.468094043444601</v>
       </c>
     </row>
     <row r="191" spans="1:4">
       <c r="A191">
-        <v>1.6642803494702</v>
+        <v>2.49792611967965</v>
       </c>
       <c r="B191">
-        <v>0.9929812715029226</v>
+        <v>3.034142169378323</v>
       </c>
       <c r="C191">
-        <v>3.046327479295549</v>
+        <v>5.166957929149434</v>
       </c>
       <c r="D191">
-        <v>2.477110284373053</v>
+        <v>6.453140926449029</v>
       </c>
     </row>
     <row r="192" spans="1:4">
       <c r="A192">
-        <v>1.752091001503925</v>
+        <v>1.918959999999999</v>
       </c>
       <c r="B192">
-        <v>0.7225000000000003</v>
+        <v>3.890859328380375</v>
       </c>
       <c r="C192">
-        <v>1.816478753448102</v>
+        <v>2.87843999999999</v>
       </c>
       <c r="D192">
-        <v>2.157099931312954</v>
+        <v>5.483839296081258</v>
       </c>
     </row>
     <row r="193" spans="1:4">
       <c r="A193">
-        <v>1.609404275953305</v>
+        <v>0.7675839999999987</v>
       </c>
       <c r="B193">
-        <v>2.096150883423502</v>
+        <v>3.459454337782194</v>
       </c>
       <c r="C193">
-        <v>2.154078818324794</v>
+        <v>0.6059873684210525</v>
       </c>
       <c r="D193">
-        <v>1.652633930510522</v>
+        <v>2.997511343615587</v>
       </c>
     </row>
     <row r="194" spans="1:4">
       <c r="A194">
-        <v>1.736673864348491</v>
+        <v>1.087410666666664</v>
       </c>
       <c r="B194">
-        <v>2.545952380952384</v>
+        <v>11.51376000000006</v>
       </c>
       <c r="C194">
-        <v>2.246860130147052</v>
+        <v>0.8937663799680083</v>
       </c>
       <c r="D194">
-        <v>1.911864910929052</v>
+        <v>2.302751999999996</v>
       </c>
     </row>
     <row r="195" spans="1:4">
       <c r="A195">
-        <v>3.231118227487202</v>
+        <v>1.415049121694472</v>
       </c>
       <c r="B195">
-        <v>2.265959829321279</v>
+        <v>8.141457772954467</v>
       </c>
       <c r="C195">
-        <v>2.157904893841293</v>
+        <v>1.106479820545486</v>
       </c>
       <c r="D195">
-        <v>2.644832987329107</v>
+        <v>0.6772799999999994</v>
       </c>
     </row>
     <row r="196" spans="1:4">
       <c r="A196">
-        <v>3.169132412822144</v>
+        <v>2.024180412912608</v>
       </c>
       <c r="B196">
-        <v>2.154078818324814</v>
+        <v>1.918959999999999</v>
       </c>
       <c r="C196">
-        <v>2.817006589175255</v>
+        <v>2.024180412912607</v>
       </c>
       <c r="D196">
-        <v>2.320013888847318</v>
+        <v>0.9794632412141231</v>
       </c>
     </row>
     <row r="197" spans="1:4">
       <c r="A197">
-        <v>3.345763594125815</v>
+        <v>1.233358028107911</v>
       </c>
       <c r="B197">
-        <v>2.154078818324792</v>
+        <v>1.132763508347406</v>
       </c>
       <c r="C197">
-        <v>2.737036662970459</v>
+        <v>2.054080746417212</v>
       </c>
       <c r="D197">
-        <v>2.880072110818022</v>
+        <v>1.23848110314451</v>
       </c>
     </row>
     <row r="198" spans="1:4">
       <c r="A198">
-        <v>3.145250140202601</v>
+        <v>3.93386800000002</v>
       </c>
       <c r="B198">
-        <v>4.816666666666673</v>
+        <v>1.002039949041459</v>
       </c>
       <c r="C198">
-        <v>2.724718130172168</v>
+        <v>2.082996921116665</v>
       </c>
       <c r="D198">
-        <v>2.724935334375981</v>
+        <v>2.022761446252248</v>
       </c>
     </row>
     <row r="199" spans="1:4">
       <c r="A199">
-        <v>2.29790844513489</v>
+        <v>1.151376</v>
       </c>
       <c r="B199">
-        <v>4.308157636649611</v>
+        <v>1.155638668797045</v>
       </c>
       <c r="C199">
-        <v>1.926666666666674</v>
+        <v>1.279306666666666</v>
       </c>
       <c r="D199">
-        <v>2.450237482127166</v>
+        <v>1.481058017666372</v>
       </c>
     </row>
     <row r="200" spans="1:4">
       <c r="A200">
-        <v>1.444999999999999</v>
+        <v>1.657623228072321</v>
       </c>
       <c r="B200">
-        <v>5.780000000000022</v>
+        <v>0.9328558038693996</v>
       </c>
       <c r="C200">
-        <v>0.8257142857142866</v>
+        <v>5.836288992570566</v>
       </c>
       <c r="D200">
-        <v>1.651428571428573</v>
+        <v>2.690002121789082</v>
       </c>
     </row>
     <row r="201" spans="1:4">
       <c r="A201">
-        <v>1.050909090909093</v>
+        <v>1.745082637497908</v>
       </c>
       <c r="B201">
-        <v>1.048075441711751</v>
+        <v>1.085527703060589</v>
       </c>
       <c r="C201">
-        <v>1.219076071111074</v>
+        <v>3.034142169378347</v>
       </c>
       <c r="D201">
-        <v>0.9248000000000014</v>
+        <v>1.211974736842105</v>
       </c>
     </row>
     <row r="202" spans="1:4">
       <c r="A202">
-        <v>1.511484779193107</v>
+        <v>1.716370002441199</v>
       </c>
       <c r="B202">
-        <v>1.143113392576158</v>
+        <v>1.041280185703051</v>
       </c>
       <c r="C202">
-        <v>2.199409674981608</v>
+        <v>1.809212838434317</v>
       </c>
       <c r="D202">
-        <v>1.34885038513884</v>
+        <v>2.467201843235556</v>
       </c>
     </row>
     <row r="203" spans="1:4">
       <c r="A203">
-        <v>1.968349358974354</v>
+        <v>1.628291554590888</v>
       </c>
       <c r="B203">
-        <v>1.615848805349964</v>
+        <v>0.9594799999999996</v>
       </c>
       <c r="C203">
-        <v>2.451010625126131</v>
+        <v>2.145462503051509</v>
       </c>
       <c r="D203">
-        <v>2.019158730105107</v>
+        <v>2.148471531587695</v>
       </c>
     </row>
     <row r="204" spans="1:4">
       <c r="A204">
-        <v>2.930419580419591</v>
+        <v>5.870888691482437</v>
       </c>
       <c r="B204">
-        <v>1.280913339563249</v>
+        <v>2.0877662798898</v>
       </c>
       <c r="C204">
-        <v>2.062330066683913</v>
+        <v>2.23787268962648</v>
       </c>
       <c r="D204">
-        <v>2.642973364622809</v>
+        <v>1.693611977428495</v>
       </c>
     </row>
     <row r="205" spans="1:4">
       <c r="A205">
-        <v>2.470723057713173</v>
+        <v>4.507769380126295</v>
       </c>
       <c r="B205">
-        <v>1.423159952359534</v>
+        <v>2.535768571428566</v>
       </c>
       <c r="C205">
-        <v>2.94723327885664</v>
+        <v>2.149273274265927</v>
       </c>
       <c r="D205">
-        <v>3.131650804487773</v>
+        <v>1.779591671416563</v>
       </c>
     </row>
     <row r="206" spans="1:4">
       <c r="A206">
-        <v>2.947233278856615</v>
+        <v>3.332380539749339</v>
       </c>
       <c r="B206">
-        <v>1.2592214809148</v>
+        <v>2.256895990003998</v>
       </c>
       <c r="C206">
-        <v>4.816666666666673</v>
+        <v>2.805738562818563</v>
       </c>
       <c r="D206">
-        <v>5.152207514416011</v>
+        <v>3.100174757489665</v>
       </c>
     </row>
     <row r="207" spans="1:4">
       <c r="A207">
-        <v>3.371666666666667</v>
+        <v>3.132669139641791</v>
       </c>
       <c r="B207">
-        <v>5.780000000000022</v>
+        <v>2.145462503051488</v>
       </c>
       <c r="C207">
-        <v>3.112625258523753</v>
+        <v>2.726088516318575</v>
       </c>
       <c r="D207">
-        <v>3.853333333333336</v>
+        <v>4.507769380126294</v>
       </c>
     </row>
     <row r="208" spans="1:4">
       <c r="A208">
-        <v>1.850502904618088</v>
+        <v>2.288716811354353</v>
       </c>
       <c r="B208">
-        <v>5.780000000000022</v>
+        <v>2.145462503051507</v>
       </c>
       <c r="C208">
-        <v>2.724718130172165</v>
+        <v>4.551213254067555</v>
       </c>
       <c r="D208">
-        <v>2.246860130147072</v>
+        <v>4.604282277769033</v>
       </c>
     </row>
     <row r="209" spans="1:4">
       <c r="A209">
-        <v>2.384128363900634</v>
+        <v>1.439220000000001</v>
       </c>
       <c r="B209">
-        <v>5.780000000000022</v>
+        <v>4.995852239359283</v>
       </c>
       <c r="C209">
-        <v>2.752931373534823</v>
+        <v>1.918959999999999</v>
       </c>
       <c r="D209">
-        <v>3.275333333333311</v>
+        <v>2.714035593038458</v>
       </c>
     </row>
     <row r="210" spans="1:4">
       <c r="A210">
-        <v>2.773800582450336</v>
+        <v>1.046705454545453</v>
       </c>
       <c r="B210">
-        <v>1.284444444444447</v>
+        <v>4.290925006102989</v>
       </c>
       <c r="C210">
-        <v>1.651428571428573</v>
+        <v>0.8224114285714289</v>
       </c>
       <c r="D210">
-        <v>3.066033784147327</v>
+        <v>7.284407964253443</v>
       </c>
     </row>
     <row r="211" spans="1:4">
       <c r="A211">
-        <v>1.651428571428573</v>
+        <v>1.505438840076331</v>
       </c>
       <c r="B211">
-        <v>1.277356643975802</v>
+        <v>6.436387509154529</v>
       </c>
       <c r="C211">
-        <v>1.284444444444447</v>
+        <v>1.214199766826632</v>
       </c>
       <c r="D211">
-        <v>1.651428571428573</v>
+        <v>1.644822857142858</v>
       </c>
     </row>
     <row r="212" spans="1:4">
       <c r="A212">
-        <v>1.651428571428573</v>
+        <v>1.964336130441083</v>
       </c>
       <c r="B212">
-        <v>1.388005463716357</v>
+        <v>11.51376000000006</v>
       </c>
       <c r="C212">
-        <v>1.249107576182414</v>
+        <v>2.19061203628171</v>
       </c>
       <c r="D212">
-        <v>1.445000000000002</v>
+        <v>0.9211007999999998</v>
       </c>
     </row>
     <row r="213" spans="1:4">
       <c r="A213">
-        <v>1.783747873651815</v>
+        <v>4.346692608234111</v>
       </c>
       <c r="B213">
-        <v>1.628438185435137</v>
+        <v>11.51376000000006</v>
       </c>
       <c r="C213">
-        <v>2.912154959912537</v>
+        <v>2.441206582625637</v>
       </c>
       <c r="D213">
-        <v>1.46107760972366</v>
+        <v>1.343454983598284</v>
       </c>
     </row>
     <row r="214" spans="1:4">
       <c r="A214">
-        <v>1.379023538916891</v>
+        <v>3.635912798685351</v>
       </c>
       <c r="B214">
-        <v>1.478033887512542</v>
+        <v>1.0438831399449</v>
       </c>
       <c r="C214">
-        <v>1.40590873416679</v>
+        <v>2.930424792355365</v>
       </c>
       <c r="D214">
-        <v>3.104434107407661</v>
+        <v>2.012555680220231</v>
       </c>
     </row>
     <row r="215" spans="1:4">
       <c r="A215">
-        <v>2.025671776025852</v>
+        <v>5.767443091451423</v>
       </c>
       <c r="B215">
-        <v>1.322416493664552</v>
+        <v>1.23454961821185</v>
       </c>
       <c r="C215">
-        <v>1.022615384615384</v>
+        <v>5.769658883648509</v>
       </c>
       <c r="D215">
-        <v>1.652676865076102</v>
+        <v>2.917351757870409</v>
       </c>
     </row>
     <row r="216" spans="1:4">
       <c r="A216">
-        <v>2.062330066683945</v>
+        <v>2.878440000000003</v>
       </c>
       <c r="B216">
-        <v>1.227512533707157</v>
+        <v>1.524107267641246</v>
       </c>
       <c r="C216">
-        <v>1.156</v>
+        <v>4.797399999999989</v>
       </c>
       <c r="D216">
-        <v>2.66425484451907</v>
+        <v>2.92788540543185</v>
       </c>
     </row>
     <row r="217" spans="1:4">
       <c r="A217">
-        <v>2.947233278856615</v>
+        <v>1.843100892999616</v>
       </c>
       <c r="B217">
-        <v>1.132979914660639</v>
+        <v>1.308563525261115</v>
       </c>
       <c r="C217">
-        <v>3.853333333333324</v>
+        <v>3.100174757489615</v>
       </c>
       <c r="D217">
-        <v>3.896442194846179</v>
+        <v>5.130264207966744</v>
       </c>
     </row>
     <row r="218" spans="1:4">
       <c r="A218">
-        <v>3.853333333333324</v>
+        <v>2.374591850445044</v>
       </c>
       <c r="B218">
-        <v>1.985962543005835</v>
+        <v>1.407042834761987</v>
       </c>
       <c r="C218">
-        <v>1.736673864348481</v>
+        <v>2.805738562818539</v>
       </c>
       <c r="D218">
-        <v>3.853333333333324</v>
+        <v>3.563782857142845</v>
       </c>
     </row>
     <row r="219" spans="1:4">
       <c r="A219">
-        <v>2.043538597629112</v>
+        <v>3.18813364853907</v>
       </c>
       <c r="B219">
-        <v>3.853333333333324</v>
+        <v>1.254184594991141</v>
       </c>
       <c r="C219">
-        <v>3.231118227487202</v>
+        <v>2.741919648040658</v>
       </c>
       <c r="D219">
-        <v>1.850502904618088</v>
+        <v>2.237872689626456</v>
       </c>
     </row>
     <row r="220" spans="1:4">
       <c r="A220">
-        <v>2.408333333333325</v>
+        <v>1.644822857142858</v>
       </c>
       <c r="B220">
-        <v>2.312</v>
+        <v>8.635320000000021</v>
       </c>
       <c r="C220">
-        <v>1.185479489419666</v>
+        <v>5.815326980681761</v>
       </c>
       <c r="D220">
-        <v>2.726420547164355</v>
+        <v>3.29281706922472</v>
       </c>
     </row>
     <row r="221" spans="1:4">
       <c r="A221">
-        <v>1.950535436429125</v>
+        <v>1.644822857142858</v>
       </c>
       <c r="B221">
-        <v>2.312</v>
+        <v>5.756879999999929</v>
       </c>
       <c r="C221">
-        <v>1.974513447704995</v>
+        <v>1.279306666666663</v>
       </c>
       <c r="D221">
-        <v>1.472250484864723</v>
+        <v>3.247252527096498</v>
       </c>
     </row>
     <row r="222" spans="1:4">
       <c r="A222">
-        <v>0.7170676691729321</v>
+        <v>1.77661288215721</v>
       </c>
       <c r="B222">
-        <v>1.050909090909091</v>
+        <v>6.918908675564385</v>
       </c>
       <c r="C222">
-        <v>0.7706666666666667</v>
+        <v>1.244111145877685</v>
       </c>
       <c r="D222">
-        <v>2.608648513551748</v>
+        <v>11.54309446792565</v>
       </c>
     </row>
     <row r="223" spans="1:4">
       <c r="A223">
-        <v>0.8257142857142845</v>
+        <v>3.856189450118902</v>
       </c>
       <c r="B223">
-        <v>2.592663174516945</v>
+        <v>8.141457772954467</v>
       </c>
       <c r="C223">
-        <v>2.246860130147052</v>
+        <v>2.900506340072891</v>
       </c>
       <c r="D223">
-        <v>0.7972413793103443</v>
+        <v>1.439219999999998</v>
       </c>
     </row>
     <row r="224" spans="1:4">
       <c r="A224">
-        <v>5.77999999999997</v>
+        <v>5.775813120641317</v>
       </c>
       <c r="B224">
-        <v>0.7266700645520283</v>
+        <v>11.51376000000006</v>
       </c>
       <c r="C224">
-        <v>2.246860130147052</v>
+        <v>3.863686839386753</v>
       </c>
       <c r="D224">
-        <v>7.706666666666741</v>
+        <v>1.455233299284766</v>
       </c>
     </row>
     <row r="225" spans="1:4">
       <c r="A225">
-        <v>3.231118227487205</v>
+        <v>3.907233056473853</v>
       </c>
       <c r="B225">
-        <v>1.062500000000001</v>
+        <v>1.279306666666663</v>
       </c>
       <c r="C225">
-        <v>1.651428571428569</v>
+        <v>2.032143023521637</v>
       </c>
       <c r="D225">
-        <v>2.644832987329104</v>
+        <v>3.092016370978037</v>
       </c>
     </row>
     <row r="226" spans="1:4">
       <c r="A226">
-        <v>3.231118227487205</v>
+        <v>2.935444345741194</v>
       </c>
       <c r="B226">
-        <v>1.878500000000001</v>
+        <v>1.272247217399901</v>
       </c>
       <c r="C226">
-        <v>1.651428571428569</v>
+        <v>5.780619812056848</v>
       </c>
       <c r="D226">
-        <v>2.644832987329104</v>
+        <v>4.34166264210809</v>
       </c>
     </row>
     <row r="227" spans="1:4">
       <c r="A227">
-        <v>1.926666666666668</v>
+        <v>2.878440000000003</v>
       </c>
       <c r="B227">
-        <v>2.600999999999993</v>
+        <v>1.518135309684449</v>
       </c>
       <c r="C227">
-        <v>2.408333333333338</v>
+        <v>3.837919999999998</v>
       </c>
       <c r="D227">
-        <v>1.778461538461533</v>
+        <v>2.652442358395757</v>
       </c>
     </row>
     <row r="228" spans="1:4">
       <c r="A228">
-        <v>3.046327479295525</v>
+        <v>1.843100892999616</v>
       </c>
       <c r="B228">
-        <v>2.889999999999985</v>
+        <v>1.758761298540484</v>
       </c>
       <c r="C228">
-        <v>2.872105091099733</v>
+        <v>2.237872689626475</v>
       </c>
       <c r="D228">
-        <v>3.954606066187226</v>
+        <v>3.876884653787841</v>
       </c>
     </row>
     <row r="229" spans="1:4">
       <c r="A229">
-        <v>2.408333333333338</v>
+        <v>3.100174757489662</v>
       </c>
       <c r="B229">
-        <v>1.156</v>
+        <v>1.472121751962497</v>
       </c>
       <c r="C229">
-        <v>2.324509559981293</v>
+        <v>3.459454337782164</v>
       </c>
       <c r="D229">
-        <v>2.335472683004714</v>
+        <v>3.289645714285716</v>
       </c>
     </row>
     <row r="230" spans="1:4">
       <c r="A230">
-        <v>2.445509363994073</v>
+        <v>1.942733294683423</v>
       </c>
       <c r="B230">
-        <v>2.091362370599074</v>
+        <v>1.317126827689893</v>
       </c>
       <c r="C230">
-        <v>2.671405144197424</v>
+        <v>1.180737571461985</v>
       </c>
       <c r="D230">
-        <v>2.627206531610715</v>
+        <v>1.925611527743263</v>
       </c>
     </row>
     <row r="231" spans="1:4">
       <c r="A231">
-        <v>2.808575162683822</v>
+        <v>3.867341786763889</v>
       </c>
       <c r="B231">
-        <v>1.520378127827915</v>
+        <v>11.51376000000006</v>
       </c>
       <c r="C231">
-        <v>3.112625258523753</v>
+        <v>1.966615393914145</v>
       </c>
       <c r="D231">
-        <v>2.520722222222221</v>
+        <v>3.218193754577213</v>
       </c>
     </row>
     <row r="232" spans="1:4">
       <c r="A232">
-        <v>2.808575162683822</v>
+        <v>5.771547233962621</v>
       </c>
       <c r="B232">
-        <v>1.156</v>
+        <v>11.51376000000006</v>
       </c>
       <c r="C232">
-        <v>1.926666666666668</v>
+        <v>5.769658883648323</v>
       </c>
       <c r="D232">
-        <v>2.644832987329105</v>
+        <v>1.466361482925266</v>
       </c>
     </row>
     <row r="233" spans="1:4">
       <c r="A233">
-        <v>2.408333333333329</v>
+        <v>5.75687999999998</v>
       </c>
       <c r="B233">
-        <v>0.9082393767240541</v>
+        <v>1.222602483572326</v>
       </c>
       <c r="C233">
-        <v>1.926666666666665</v>
+        <v>11.51376000000006</v>
       </c>
       <c r="D233">
-        <v>2.644832987329107</v>
+        <v>2.59821391949753</v>
       </c>
     </row>
     <row r="234" spans="1:4">
       <c r="A234">
-        <v>1.926666666666668</v>
+        <v>3.218193754577239</v>
       </c>
       <c r="B234">
-        <v>1.467936507936509</v>
+        <v>1.128447995001998</v>
       </c>
       <c r="C234">
-        <v>2.119333333333331</v>
+        <v>2.035364443238608</v>
       </c>
       <c r="D234">
-        <v>1.926666666666668</v>
+        <v>5.770554318552234</v>
       </c>
     </row>
     <row r="235" spans="1:4">
       <c r="A235">
-        <v>2.389204774980597</v>
+        <v>3.218193754577239</v>
       </c>
       <c r="B235">
-        <v>1.981714285714287</v>
+        <v>1.978018692833826</v>
       </c>
       <c r="C235">
-        <v>2.312</v>
+        <v>1.843100892999624</v>
       </c>
       <c r="D235">
-        <v>2.898685550490111</v>
+        <v>7.675840000000042</v>
       </c>
     </row>
     <row r="236" spans="1:4">
       <c r="A236">
-        <v>2.312</v>
+        <v>5.836288992570466</v>
       </c>
       <c r="B236">
-        <v>2.600999999999993</v>
+        <v>3.837919999999998</v>
       </c>
       <c r="C236">
-        <v>2.445509363994073</v>
+        <v>1.644822857142858</v>
       </c>
       <c r="D236">
-        <v>2.20690909090909</v>
+        <v>2.3987</v>
       </c>
     </row>
     <row r="237" spans="1:4">
       <c r="A237">
-        <v>2.312</v>
+        <v>3.034142169378347</v>
       </c>
       <c r="B237">
-        <v>2.889999999999985</v>
+        <v>5.934056078501285</v>
       </c>
       <c r="C237">
-        <v>2.659654995379001</v>
+        <v>7.69539631195016</v>
       </c>
       <c r="D237">
-        <v>2.312</v>
+        <v>2.306302891854793</v>
       </c>
     </row>
     <row r="238" spans="1:4">
       <c r="A238">
-        <v>3.458472509470822</v>
+        <v>2.3987</v>
       </c>
       <c r="B238">
-        <v>2.94723327885664</v>
+        <v>2.878440000000015</v>
       </c>
       <c r="C238">
-        <v>3.971925086011677</v>
+        <v>2.3987</v>
       </c>
       <c r="D238">
-        <v>2.862476190476185</v>
+        <v>11.54777413614213</v>
       </c>
     </row>
     <row r="239" spans="1:4">
       <c r="A239">
-        <v>2.900017361059149</v>
+        <v>2.435727326538102</v>
       </c>
       <c r="B239">
-        <v>1.156</v>
+        <v>5.780619812056849</v>
       </c>
       <c r="C239">
-        <v>3.929644371808836</v>
+        <v>2.732600237852421</v>
       </c>
       <c r="D239">
-        <v>2.579613892956597</v>
+        <v>10.2514713737246</v>
       </c>
     </row>
     <row r="240" spans="1:4">
       <c r="A240">
-        <v>3.352498423416836</v>
+        <v>2.797340862033081</v>
       </c>
       <c r="B240">
-        <v>1.156</v>
+        <v>2.582292521818875</v>
       </c>
       <c r="C240">
-        <v>3.112625258523753</v>
+        <v>2.3987</v>
       </c>
       <c r="D240">
-        <v>3.599310366043913</v>
+        <v>2.326130792272693</v>
       </c>
     </row>
     <row r="241" spans="1:4">
       <c r="A241">
-        <v>3.352498423416836</v>
+        <v>2.797340862033081</v>
       </c>
       <c r="B241">
-        <v>1.284444444444444</v>
+        <v>0.6585634138449472</v>
       </c>
       <c r="C241">
-        <v>1.926666666666668</v>
+        <v>2.660719523620638</v>
       </c>
       <c r="D241">
-        <v>3.572151641105233</v>
+        <v>2.562282182505389</v>
       </c>
     </row>
     <row r="242" spans="1:4">
       <c r="A242">
-        <v>2.408333333333329</v>
+        <v>2.398699999999996</v>
       </c>
       <c r="B242">
-        <v>1.364722222222222</v>
+        <v>3.899976975340095</v>
       </c>
       <c r="C242">
-        <v>2.408333333333333</v>
+        <v>3.100174757489663</v>
       </c>
       <c r="D242">
-        <v>2.644832987329107</v>
+        <v>2.554812568689921</v>
       </c>
     </row>
     <row r="243" spans="1:4">
       <c r="A243">
-        <v>3.231118227487182</v>
+        <v>1.918959999999999</v>
       </c>
       <c r="B243">
-        <v>1.444999999999999</v>
+        <v>4.035523149156144</v>
       </c>
       <c r="C243">
-        <v>2.889999999999998</v>
+        <v>1.644822857142858</v>
       </c>
       <c r="D243">
-        <v>4.022998108100147</v>
+        <v>2.634253655379786</v>
       </c>
     </row>
     <row r="244" spans="1:4">
       <c r="A244">
-        <v>2.600999999999999</v>
+        <v>4.444785274766797</v>
+      </c>
+      <c r="B244">
+        <v>2.590595999999993</v>
       </c>
       <c r="C244">
-        <v>3.853333333333347</v>
+        <v>4.017561692680811</v>
       </c>
       <c r="D244">
-        <v>2.440444444444447</v>
+        <v>2.634253655379784</v>
       </c>
     </row>
     <row r="245" spans="1:4">
       <c r="A245">
-        <v>2.312</v>
+        <v>4.13356634331955</v>
+      </c>
+      <c r="B245">
+        <v>2.87843999999999</v>
       </c>
       <c r="C245">
-        <v>3.45847250947082</v>
+        <v>4.087780184736855</v>
       </c>
       <c r="D245">
-        <v>2.568888888888893</v>
+        <v>1.771347692307687</v>
       </c>
     </row>
     <row r="246" spans="1:4">
       <c r="A246">
-        <v>3.853333333333347</v>
+        <v>2.302751999999996</v>
+      </c>
+      <c r="B246">
+        <v>1.151376</v>
       </c>
       <c r="C246">
-        <v>3.11262525852373</v>
+        <v>2.302752000000004</v>
       </c>
       <c r="D246">
-        <v>3.853333333333347</v>
+        <v>7.736410158855374</v>
       </c>
     </row>
     <row r="247" spans="1:4">
       <c r="A247">
-        <v>3.211111111111106</v>
+        <v>3.444638619432951</v>
+      </c>
+      <c r="B247">
+        <v>4.360212324500632</v>
+      </c>
+      <c r="C247">
+        <v>2.578525021445831</v>
       </c>
       <c r="D247">
-        <v>3.21880855190662</v>
+        <v>1.099040727272727</v>
       </c>
     </row>
     <row r="248" spans="1:4">
       <c r="A248">
-        <v>3.473347728696983</v>
+        <v>2.888417291614904</v>
+      </c>
+      <c r="B248">
+        <v>3.885729476626909</v>
+      </c>
+      <c r="C248">
+        <v>2.3987</v>
       </c>
       <c r="D248">
-        <v>2.841225145343218</v>
+        <v>2.302751999999996</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4">
+      <c r="A249">
+        <v>3.339088429723158</v>
+      </c>
+      <c r="B249">
+        <v>5.785592796571874</v>
+      </c>
+      <c r="C249">
+        <v>3.339088429723175</v>
+      </c>
+      <c r="D249">
+        <v>2.926184830066203</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4">
+      <c r="A250">
+        <v>3.339088429723165</v>
+      </c>
+      <c r="B250">
+        <v>0.8605655467124195</v>
+      </c>
+      <c r="C250">
+        <v>3.913925794321608</v>
+      </c>
+      <c r="D250">
+        <v>2.54985307610066</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4">
+      <c r="A251">
+        <v>2.398700000000006</v>
+      </c>
+      <c r="B251">
+        <v>0.7310323809523825</v>
+      </c>
+      <c r="C251">
+        <v>3.10017475748964</v>
+      </c>
+      <c r="D251">
+        <v>3.339088429723158</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4">
+      <c r="A252">
+        <v>3.218193754577262</v>
+      </c>
+      <c r="B252">
+        <v>1.973787428571429</v>
+      </c>
+      <c r="C252">
+        <v>5.870888691482436</v>
+      </c>
+      <c r="D252">
+        <v>3.557863034540807</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4">
+      <c r="A253">
+        <v>4.290925006103014</v>
+      </c>
+      <c r="B253">
+        <v>2.590595999999993</v>
+      </c>
+      <c r="C253">
+        <v>2.302752</v>
+      </c>
+      <c r="D253">
+        <v>2.634253655379798</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4">
+      <c r="A254">
+        <v>2.87843999999999</v>
+      </c>
+      <c r="B254">
+        <v>2.87843999999999</v>
+      </c>
+      <c r="C254">
+        <v>2.302752000000004</v>
+      </c>
+      <c r="D254">
+        <v>4.045522892504537</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4">
+      <c r="A255">
+        <v>3.837919999999998</v>
+      </c>
+      <c r="B255">
+        <v>2.935444345741193</v>
+      </c>
+      <c r="C255">
+        <v>3.837919999999998</v>
+      </c>
+      <c r="D255">
+        <v>7.86308312522971</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4">
+      <c r="A256">
+        <v>3.198266666666678</v>
+      </c>
+      <c r="B256">
+        <v>3.913925794321624</v>
+      </c>
+      <c r="C256">
+        <v>3.444638619432935</v>
+      </c>
+      <c r="D256">
+        <v>2.558613333333327</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4">
+      <c r="A257">
+        <v>3.459454337782186</v>
+      </c>
+      <c r="B257">
+        <v>5.785592796571874</v>
+      </c>
+      <c r="C257">
+        <v>3.218193754577239</v>
+      </c>
+      <c r="D257">
+        <v>3.837919999999975</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4">
+      <c r="B258">
+        <v>1.279306666666666</v>
+      </c>
+      <c r="D258">
+        <v>3.205933317698993</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4">
+      <c r="B259">
+        <v>1.359263333333334</v>
+      </c>
+      <c r="D259">
+        <v>2.997511343615575</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4">
+      <c r="B260">
+        <v>5.80168129825315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>